<commit_message>
small code fixes - removed dc-ac on pv inputs
</commit_message>
<xml_diff>
--- a/(client deliverable)SGWS_Scenario_comparison.xlsx
+++ b/(client deliverable)SGWS_Scenario_comparison.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mykolaturchak/PycharmProjects/Valuestack/sgws_microgrid/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{B4F52545-9A46-834E-8DE8-2AED1AC6D0F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE18ACD4-C135-9C4C-8046-FD538DBC4AAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="160" yWindow="660" windowWidth="28480" windowHeight="16120" xr2:uid="{BBC9B5F1-E85E-E64A-A67A-0CEF0D7F3E37}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="18">
   <si>
     <t>total_load_kwh</t>
   </si>
@@ -75,9 +75,6 @@
   </si>
   <si>
     <t>Solar_kw_DC</t>
-  </si>
-  <si>
-    <t>Solar_kw_AC</t>
   </si>
   <si>
     <t>EV_load_scenario</t>
@@ -573,10 +570,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -952,20 +948,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CC78E7F-F823-9A45-863E-EBED49755FF5}">
-  <dimension ref="A1:P67"/>
+  <dimension ref="A1:O67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="K45" sqref="K45"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="I52" sqref="I52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="17" max="17" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="13.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -976,3408 +972,3141 @@
         <v>14</v>
       </c>
       <c r="D1" t="s">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="E1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="J1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="K1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="L1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="M1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="N1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="O1" t="s">
-        <v>10</v>
-      </c>
-      <c r="P1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>100</v>
       </c>
       <c r="B2">
         <v>259.2</v>
       </c>
-      <c r="C2" s="2">
-        <f>B2/1.4</f>
-        <v>185.14285714285714</v>
-      </c>
-      <c r="D2" t="s">
-        <v>16</v>
+      <c r="C2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2">
+        <v>135543.5</v>
       </c>
       <c r="E2">
-        <v>135543.5</v>
+        <v>392886.42</v>
       </c>
       <c r="F2">
-        <v>391640.86</v>
+        <v>264576.46999999997</v>
       </c>
       <c r="G2">
-        <v>263171</v>
+        <v>128309.95</v>
       </c>
       <c r="H2">
-        <v>128469.86</v>
+        <v>9229.33</v>
       </c>
       <c r="I2">
-        <v>9063.51</v>
+        <v>93</v>
       </c>
       <c r="J2">
-        <v>93</v>
+        <v>33</v>
       </c>
       <c r="K2">
-        <v>33</v>
+        <v>25946.2</v>
       </c>
       <c r="L2">
-        <v>25870.76</v>
+        <v>23950.41</v>
       </c>
       <c r="M2">
-        <v>23880.89</v>
+        <v>124.54</v>
       </c>
       <c r="N2">
-        <v>124.18</v>
+        <v>3261</v>
       </c>
       <c r="O2">
-        <v>3223</v>
-      </c>
-      <c r="P2">
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>200</v>
       </c>
       <c r="B3">
         <v>259.2</v>
       </c>
-      <c r="C3" s="2">
-        <f t="shared" ref="C3:C66" si="0">B3/1.4</f>
-        <v>185.14285714285714</v>
-      </c>
-      <c r="D3" t="s">
-        <v>16</v>
+      <c r="C3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3">
+        <v>135543.5</v>
       </c>
       <c r="E3">
-        <v>135543.5</v>
+        <v>392886.42</v>
       </c>
       <c r="F3">
-        <v>391640.86</v>
+        <v>257055.69</v>
       </c>
       <c r="G3">
-        <v>255762.66</v>
+        <v>135830.73000000001</v>
       </c>
       <c r="H3">
-        <v>135878.20000000001</v>
+        <v>2324.31</v>
       </c>
       <c r="I3">
-        <v>2262.91</v>
+        <v>98</v>
       </c>
       <c r="J3">
-        <v>98</v>
+        <v>35</v>
       </c>
       <c r="K3">
-        <v>35</v>
+        <v>33466.980000000003</v>
       </c>
       <c r="L3">
-        <v>33279.1</v>
+        <v>30855.439999999999</v>
       </c>
       <c r="M3">
-        <v>30681.49</v>
+        <v>80.319999999999993</v>
       </c>
       <c r="N3">
-        <v>79.87</v>
+        <v>653</v>
       </c>
       <c r="O3">
-        <v>634</v>
-      </c>
-      <c r="P3">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>300</v>
       </c>
       <c r="B4">
         <v>259.2</v>
       </c>
-      <c r="C4" s="2">
-        <f t="shared" si="0"/>
-        <v>185.14285714285714</v>
-      </c>
-      <c r="D4" t="s">
-        <v>16</v>
+      <c r="C4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4">
+        <v>135543.5</v>
       </c>
       <c r="E4">
-        <v>135543.5</v>
+        <v>392886.42</v>
       </c>
       <c r="F4">
-        <v>391640.86</v>
+        <v>255348.54</v>
       </c>
       <c r="G4">
-        <v>254085.7</v>
+        <v>137537.88</v>
       </c>
       <c r="H4">
-        <v>137555.16</v>
+        <v>799</v>
       </c>
       <c r="I4">
-        <v>765.42</v>
+        <v>99</v>
       </c>
       <c r="J4">
-        <v>99</v>
+        <v>35</v>
       </c>
       <c r="K4">
-        <v>35</v>
+        <v>35174.129999999997</v>
       </c>
       <c r="L4">
-        <v>34956.06</v>
+        <v>32380.75</v>
       </c>
       <c r="M4">
-        <v>32178.98</v>
+        <v>56.22</v>
       </c>
       <c r="N4">
-        <v>55.87</v>
+        <v>215</v>
       </c>
       <c r="O4">
-        <v>202</v>
-      </c>
-      <c r="P4">
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>400</v>
       </c>
       <c r="B5">
         <v>259.2</v>
       </c>
-      <c r="C5" s="2">
-        <f t="shared" si="0"/>
-        <v>185.14285714285714</v>
-      </c>
-      <c r="D5" t="s">
-        <v>16</v>
+      <c r="C5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5">
+        <v>135543.5</v>
       </c>
       <c r="E5">
-        <v>135543.5</v>
+        <v>392886.42</v>
       </c>
       <c r="F5">
-        <v>391640.86</v>
+        <v>254807.99</v>
       </c>
       <c r="G5">
-        <v>253569.92000000001</v>
+        <v>138078.43</v>
       </c>
       <c r="H5">
-        <v>138070.94</v>
+        <v>348.83</v>
       </c>
       <c r="I5">
-        <v>338.08</v>
+        <v>100</v>
       </c>
       <c r="J5">
-        <v>100</v>
+        <v>35</v>
       </c>
       <c r="K5">
-        <v>35</v>
+        <v>35714.68</v>
       </c>
       <c r="L5">
-        <v>35471.839999999997</v>
+        <v>32830.92</v>
       </c>
       <c r="M5">
-        <v>32606.32</v>
+        <v>42.75</v>
       </c>
       <c r="N5">
-        <v>42.46</v>
+        <v>77</v>
       </c>
       <c r="O5">
-        <v>71</v>
-      </c>
-      <c r="P5">
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>500</v>
       </c>
       <c r="B6">
         <v>259.2</v>
       </c>
-      <c r="C6" s="2">
-        <f t="shared" si="0"/>
-        <v>185.14285714285714</v>
-      </c>
-      <c r="D6" t="s">
-        <v>16</v>
+      <c r="C6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6">
+        <v>135543.5</v>
       </c>
       <c r="E6">
-        <v>135543.5</v>
+        <v>392886.42</v>
       </c>
       <c r="F6">
-        <v>391640.86</v>
+        <v>254594.37</v>
       </c>
       <c r="G6">
-        <v>253366.14</v>
+        <v>138292.04999999999</v>
       </c>
       <c r="H6">
-        <v>138274.72</v>
+        <v>199.96</v>
       </c>
       <c r="I6">
-        <v>198.28</v>
+        <v>100</v>
       </c>
       <c r="J6">
-        <v>100</v>
+        <v>35</v>
       </c>
       <c r="K6">
-        <v>35</v>
+        <v>35928.29</v>
       </c>
       <c r="L6">
-        <v>35675.620000000003</v>
+        <v>32979.79</v>
       </c>
       <c r="M6">
-        <v>32746.12</v>
+        <v>34.35</v>
       </c>
       <c r="N6">
-        <v>34.11</v>
+        <v>32</v>
       </c>
       <c r="O6">
-        <v>32</v>
-      </c>
-      <c r="P6">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>600</v>
       </c>
       <c r="B7">
         <v>259.2</v>
       </c>
-      <c r="C7" s="2">
-        <f t="shared" si="0"/>
-        <v>185.14285714285714</v>
-      </c>
-      <c r="D7" t="s">
-        <v>16</v>
+      <c r="C7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7">
+        <v>135543.5</v>
       </c>
       <c r="E7">
-        <v>135543.5</v>
+        <v>392886.42</v>
       </c>
       <c r="F7">
-        <v>391640.86</v>
+        <v>254448.54</v>
       </c>
       <c r="G7">
-        <v>253220.31</v>
+        <v>138437.88</v>
       </c>
       <c r="H7">
-        <v>138420.54999999999</v>
+        <v>113.56</v>
       </c>
       <c r="I7">
-        <v>111.88</v>
+        <v>100</v>
       </c>
       <c r="J7">
-        <v>100</v>
+        <v>35</v>
       </c>
       <c r="K7">
-        <v>35</v>
+        <v>36074.129999999997</v>
       </c>
       <c r="L7">
-        <v>35821.449999999997</v>
+        <v>33066.19</v>
       </c>
       <c r="M7">
-        <v>32832.519999999997</v>
+        <v>28.7</v>
       </c>
       <c r="N7">
-        <v>28.5</v>
+        <v>29</v>
       </c>
       <c r="O7">
-        <v>29</v>
-      </c>
-      <c r="P7">
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>700</v>
       </c>
       <c r="B8">
         <v>259.2</v>
       </c>
-      <c r="C8" s="2">
-        <f t="shared" si="0"/>
-        <v>185.14285714285714</v>
-      </c>
-      <c r="D8" t="s">
-        <v>16</v>
+      <c r="C8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8">
+        <v>135543.5</v>
       </c>
       <c r="E8">
-        <v>135543.5</v>
+        <v>392886.42</v>
       </c>
       <c r="F8">
-        <v>391640.86</v>
+        <v>254302.71</v>
       </c>
       <c r="G8">
-        <v>253074.47</v>
+        <v>138583.71</v>
       </c>
       <c r="H8">
-        <v>138566.39000000001</v>
+        <v>27.16</v>
       </c>
       <c r="I8">
-        <v>25.48</v>
+        <v>100</v>
       </c>
       <c r="J8">
-        <v>100</v>
+        <v>35</v>
       </c>
       <c r="K8">
-        <v>35</v>
+        <v>36219.96</v>
       </c>
       <c r="L8">
-        <v>35967.29</v>
+        <v>33152.589999999997</v>
       </c>
       <c r="M8">
-        <v>32918.92</v>
+        <v>24.67</v>
       </c>
       <c r="N8">
-        <v>24.49</v>
+        <v>19</v>
       </c>
       <c r="O8">
-        <v>17</v>
-      </c>
-      <c r="P8">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>800</v>
       </c>
       <c r="B9">
         <v>259.2</v>
       </c>
-      <c r="C9" s="2">
-        <f t="shared" si="0"/>
-        <v>185.14285714285714</v>
-      </c>
-      <c r="D9" t="s">
-        <v>16</v>
+      <c r="C9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9">
+        <v>135543.5</v>
       </c>
       <c r="E9">
-        <v>135543.5</v>
+        <v>392886.42</v>
       </c>
       <c r="F9">
-        <v>391640.86</v>
+        <v>254221.15</v>
       </c>
       <c r="G9">
-        <v>252994.74</v>
+        <v>138665.26999999999</v>
       </c>
       <c r="H9">
-        <v>138646.12</v>
+        <v>0</v>
       </c>
       <c r="I9">
+        <v>100</v>
+      </c>
+      <c r="J9">
+        <v>35</v>
+      </c>
+      <c r="K9">
+        <v>36301.519999999997</v>
+      </c>
+      <c r="L9">
+        <v>33179.75</v>
+      </c>
+      <c r="M9">
+        <v>21.6</v>
+      </c>
+      <c r="N9">
         <v>0</v>
-      </c>
-      <c r="J9">
-        <v>100</v>
-      </c>
-      <c r="K9">
-        <v>35</v>
-      </c>
-      <c r="L9">
-        <v>36047.019999999997</v>
-      </c>
-      <c r="M9">
-        <v>32944.400000000001</v>
-      </c>
-      <c r="N9">
-        <v>21.45</v>
       </c>
       <c r="O9">
         <v>0</v>
       </c>
-      <c r="P9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>100</v>
       </c>
       <c r="B10">
         <v>259.2</v>
       </c>
-      <c r="C10" s="2">
-        <f t="shared" si="0"/>
-        <v>185.14285714285714</v>
-      </c>
-      <c r="D10" t="s">
-        <v>17</v>
+      <c r="C10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10">
+        <v>192783.5</v>
       </c>
       <c r="E10">
-        <v>192783.5</v>
+        <v>392886.42</v>
       </c>
       <c r="F10">
-        <v>391640.86</v>
+        <v>219553.29</v>
       </c>
       <c r="G10">
-        <v>218043.42</v>
+        <v>173333.13</v>
       </c>
       <c r="H10">
-        <v>173597.44</v>
+        <v>21647.53</v>
       </c>
       <c r="I10">
-        <v>21379.47</v>
+        <v>89</v>
       </c>
       <c r="J10">
-        <v>89</v>
+        <v>44</v>
       </c>
       <c r="K10">
-        <v>44</v>
+        <v>28514.78</v>
       </c>
       <c r="L10">
-        <v>28466.94</v>
+        <v>26317.62</v>
       </c>
       <c r="M10">
-        <v>26273.53</v>
+        <v>136.87</v>
       </c>
       <c r="N10">
-        <v>136.63999999999999</v>
+        <v>4815</v>
       </c>
       <c r="O10">
-        <v>4771</v>
-      </c>
-      <c r="P10">
         <v>36</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>200</v>
       </c>
       <c r="B11">
         <v>259.2</v>
       </c>
-      <c r="C11" s="2">
-        <f t="shared" si="0"/>
-        <v>185.14285714285714</v>
-      </c>
-      <c r="D11" t="s">
-        <v>17</v>
+      <c r="C11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11">
+        <v>192783.5</v>
       </c>
       <c r="E11">
-        <v>192783.5</v>
+        <v>392886.42</v>
       </c>
       <c r="F11">
-        <v>391640.86</v>
+        <v>206923.61</v>
       </c>
       <c r="G11">
-        <v>205480.76</v>
+        <v>185962.81</v>
       </c>
       <c r="H11">
-        <v>186160.1</v>
+        <v>9998.23</v>
       </c>
       <c r="I11">
-        <v>9792.91</v>
+        <v>95</v>
       </c>
       <c r="J11">
-        <v>95</v>
+        <v>47</v>
       </c>
       <c r="K11">
-        <v>48</v>
+        <v>41144.46</v>
       </c>
       <c r="L11">
-        <v>41029.599999999999</v>
+        <v>37966.93</v>
       </c>
       <c r="M11">
-        <v>37860.089999999997</v>
+        <v>98.75</v>
       </c>
       <c r="N11">
-        <v>98.47</v>
+        <v>2198</v>
       </c>
       <c r="O11">
-        <v>2164</v>
-      </c>
-      <c r="P11">
         <v>36</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>300</v>
       </c>
       <c r="B12">
         <v>259.2</v>
       </c>
-      <c r="C12" s="2">
-        <f t="shared" si="0"/>
-        <v>185.14285714285714</v>
-      </c>
-      <c r="D12" t="s">
-        <v>17</v>
+      <c r="C12" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12">
+        <v>192783.5</v>
       </c>
       <c r="E12">
-        <v>192783.5</v>
+        <v>392886.42</v>
       </c>
       <c r="F12">
-        <v>391640.86</v>
+        <v>202351.82</v>
       </c>
       <c r="G12">
-        <v>200983.16</v>
+        <v>190534.6</v>
       </c>
       <c r="H12">
-        <v>190657.7</v>
+        <v>5832.86</v>
       </c>
       <c r="I12">
-        <v>5695.93</v>
+        <v>97</v>
       </c>
       <c r="J12">
-        <v>97</v>
+        <v>48</v>
       </c>
       <c r="K12">
-        <v>49</v>
+        <v>45716.25</v>
       </c>
       <c r="L12">
-        <v>45527.199999999997</v>
+        <v>42132.29</v>
       </c>
       <c r="M12">
-        <v>41957.08</v>
+        <v>73.150000000000006</v>
       </c>
       <c r="N12">
-        <v>72.84</v>
+        <v>1116</v>
       </c>
       <c r="O12">
-        <v>1089</v>
-      </c>
-      <c r="P12">
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>400</v>
       </c>
       <c r="B13">
         <v>259.2</v>
       </c>
-      <c r="C13" s="2">
-        <f t="shared" si="0"/>
-        <v>185.14285714285714</v>
-      </c>
-      <c r="D13" t="s">
-        <v>17</v>
+      <c r="C13" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13">
+        <v>192783.5</v>
       </c>
       <c r="E13">
-        <v>192783.5</v>
+        <v>392886.42</v>
       </c>
       <c r="F13">
-        <v>391640.86</v>
+        <v>200267.44</v>
       </c>
       <c r="G13">
-        <v>198930.75</v>
+        <v>192618.98</v>
       </c>
       <c r="H13">
-        <v>192710.11</v>
+        <v>3959.9</v>
       </c>
       <c r="I13">
-        <v>3852.43</v>
+        <v>98</v>
       </c>
       <c r="J13">
-        <v>98</v>
+        <v>49</v>
       </c>
       <c r="K13">
-        <v>49</v>
+        <v>47800.63</v>
       </c>
       <c r="L13">
-        <v>47579.61</v>
+        <v>44005.25</v>
       </c>
       <c r="M13">
-        <v>43800.58</v>
+        <v>57.3</v>
       </c>
       <c r="N13">
-        <v>57.03</v>
+        <v>692</v>
       </c>
       <c r="O13">
-        <v>682</v>
-      </c>
-      <c r="P13">
         <v>36</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>500</v>
       </c>
       <c r="B14">
         <v>259.2</v>
       </c>
-      <c r="C14" s="2">
-        <f t="shared" si="0"/>
-        <v>185.14285714285714</v>
-      </c>
-      <c r="D14" t="s">
-        <v>17</v>
+      <c r="C14" t="s">
+        <v>16</v>
+      </c>
+      <c r="D14">
+        <v>192783.5</v>
       </c>
       <c r="E14">
-        <v>192783.5</v>
+        <v>392886.42</v>
       </c>
       <c r="F14">
-        <v>391640.86</v>
+        <v>198702.8</v>
       </c>
       <c r="G14">
-        <v>197385.24</v>
+        <v>194183.62</v>
       </c>
       <c r="H14">
-        <v>194255.62</v>
+        <v>2565.9299999999998</v>
       </c>
       <c r="I14">
-        <v>2476.08</v>
+        <v>99</v>
       </c>
       <c r="J14">
-        <v>99</v>
+        <v>49</v>
       </c>
       <c r="K14">
-        <v>50</v>
+        <v>49365.27</v>
       </c>
       <c r="L14">
-        <v>49125.120000000003</v>
+        <v>45399.22</v>
       </c>
       <c r="M14">
-        <v>45176.92</v>
+        <v>47.29</v>
       </c>
       <c r="N14">
-        <v>47.06</v>
+        <v>508</v>
       </c>
       <c r="O14">
-        <v>503</v>
-      </c>
-      <c r="P14">
         <v>36</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>600</v>
       </c>
       <c r="B15">
         <v>259.2</v>
       </c>
-      <c r="C15" s="2">
-        <f t="shared" si="0"/>
-        <v>185.14285714285714</v>
-      </c>
-      <c r="D15" t="s">
-        <v>17</v>
+      <c r="C15" t="s">
+        <v>16</v>
+      </c>
+      <c r="D15">
+        <v>192783.5</v>
       </c>
       <c r="E15">
-        <v>192783.5</v>
+        <v>392886.42</v>
       </c>
       <c r="F15">
-        <v>391640.86</v>
+        <v>197597.57</v>
       </c>
       <c r="G15">
-        <v>196308.21</v>
+        <v>195288.85</v>
       </c>
       <c r="H15">
-        <v>195332.65</v>
+        <v>1595.35</v>
       </c>
       <c r="I15">
-        <v>1531.49</v>
+        <v>99</v>
       </c>
       <c r="J15">
-        <v>99</v>
+        <v>50</v>
       </c>
       <c r="K15">
-        <v>50</v>
+        <v>50470.5</v>
       </c>
       <c r="L15">
-        <v>50202.15</v>
+        <v>46369.81</v>
       </c>
       <c r="M15">
-        <v>46121.52</v>
+        <v>40.25</v>
       </c>
       <c r="N15">
-        <v>40.04</v>
+        <v>292</v>
       </c>
       <c r="O15">
-        <v>276</v>
-      </c>
-      <c r="P15">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>700</v>
       </c>
       <c r="B16">
         <v>259.2</v>
       </c>
-      <c r="C16" s="2">
-        <f t="shared" si="0"/>
-        <v>185.14285714285714</v>
-      </c>
-      <c r="D16" t="s">
-        <v>17</v>
+      <c r="C16" t="s">
+        <v>16</v>
+      </c>
+      <c r="D16">
+        <v>192783.5</v>
       </c>
       <c r="E16">
-        <v>192783.5</v>
+        <v>392886.42</v>
       </c>
       <c r="F16">
-        <v>391640.86</v>
+        <v>196872.43</v>
       </c>
       <c r="G16">
-        <v>195613.76</v>
+        <v>196013.99</v>
       </c>
       <c r="H16">
-        <v>196027.1</v>
+        <v>975.06</v>
       </c>
       <c r="I16">
-        <v>939.48</v>
+        <v>99</v>
       </c>
       <c r="J16">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="K16">
-        <v>50</v>
+        <v>51195.64</v>
       </c>
       <c r="L16">
-        <v>50896.6</v>
+        <v>46990.1</v>
       </c>
       <c r="M16">
-        <v>46713.52</v>
+        <v>34.96</v>
       </c>
       <c r="N16">
-        <v>34.76</v>
+        <v>105</v>
       </c>
       <c r="O16">
-        <v>96</v>
-      </c>
-      <c r="P16">
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>800</v>
       </c>
       <c r="B17">
         <v>259.2</v>
       </c>
-      <c r="C17" s="2">
-        <f t="shared" si="0"/>
-        <v>185.14285714285714</v>
-      </c>
-      <c r="D17" t="s">
-        <v>17</v>
+      <c r="C17" t="s">
+        <v>16</v>
+      </c>
+      <c r="D17">
+        <v>192783.5</v>
       </c>
       <c r="E17">
-        <v>192783.5</v>
+        <v>392886.42</v>
       </c>
       <c r="F17">
-        <v>391640.86</v>
+        <v>196587.41</v>
       </c>
       <c r="G17">
-        <v>195343.07</v>
+        <v>196299.01</v>
       </c>
       <c r="H17">
-        <v>196297.79</v>
+        <v>760.38</v>
       </c>
       <c r="I17">
-        <v>738.02</v>
+        <v>100</v>
       </c>
       <c r="J17">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="K17">
-        <v>50</v>
+        <v>51480.67</v>
       </c>
       <c r="L17">
-        <v>51167.29</v>
+        <v>47204.77</v>
       </c>
       <c r="M17">
-        <v>46914.98</v>
+        <v>30.73</v>
       </c>
       <c r="N17">
-        <v>30.54</v>
+        <v>69</v>
       </c>
       <c r="O17">
-        <v>68</v>
-      </c>
-      <c r="P17">
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>900</v>
       </c>
       <c r="B18">
         <v>259.2</v>
       </c>
-      <c r="C18" s="2">
-        <f t="shared" si="0"/>
-        <v>185.14285714285714</v>
-      </c>
-      <c r="D18" t="s">
-        <v>17</v>
+      <c r="C18" t="s">
+        <v>16</v>
+      </c>
+      <c r="D18">
+        <v>192783.5</v>
       </c>
       <c r="E18">
-        <v>192783.5</v>
+        <v>392886.42</v>
       </c>
       <c r="F18">
-        <v>391640.86</v>
+        <v>196347.82</v>
       </c>
       <c r="G18">
-        <v>195103.49</v>
+        <v>196538.6</v>
       </c>
       <c r="H18">
-        <v>196537.37</v>
+        <v>587.58000000000004</v>
       </c>
       <c r="I18">
-        <v>565.22</v>
+        <v>100</v>
       </c>
       <c r="J18">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="K18">
-        <v>50</v>
+        <v>51720.25</v>
       </c>
       <c r="L18">
-        <v>51406.87</v>
+        <v>47377.57</v>
       </c>
       <c r="M18">
-        <v>47087.78</v>
+        <v>27.42</v>
       </c>
       <c r="N18">
-        <v>27.25</v>
+        <v>63</v>
       </c>
       <c r="O18">
-        <v>63</v>
-      </c>
-      <c r="P18">
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>1000</v>
       </c>
       <c r="B19">
         <v>259.2</v>
       </c>
-      <c r="C19" s="2">
-        <f t="shared" si="0"/>
-        <v>185.14285714285714</v>
-      </c>
-      <c r="D19" t="s">
+      <c r="C19" t="s">
+        <v>16</v>
+      </c>
+      <c r="D19">
+        <v>192783.5</v>
+      </c>
+      <c r="E19">
+        <v>392886.42</v>
+      </c>
+      <c r="F19">
+        <v>196108.24</v>
+      </c>
+      <c r="G19">
+        <v>196778.18</v>
+      </c>
+      <c r="H19">
+        <v>414.78</v>
+      </c>
+      <c r="I19">
+        <v>100</v>
+      </c>
+      <c r="J19">
+        <v>50</v>
+      </c>
+      <c r="K19">
+        <v>51959.83</v>
+      </c>
+      <c r="L19">
+        <v>47550.37</v>
+      </c>
+      <c r="M19">
+        <v>24.77</v>
+      </c>
+      <c r="N19">
+        <v>59</v>
+      </c>
+      <c r="O19">
         <v>17</v>
       </c>
-      <c r="E19">
-        <v>192783.5</v>
-      </c>
-      <c r="F19">
-        <v>391640.86</v>
-      </c>
-      <c r="G19">
-        <v>194863.91</v>
-      </c>
-      <c r="H19">
-        <v>196776.95</v>
-      </c>
-      <c r="I19">
-        <v>392.42</v>
-      </c>
-      <c r="J19">
-        <v>100</v>
-      </c>
-      <c r="K19">
-        <v>50</v>
-      </c>
-      <c r="L19">
-        <v>51646.46</v>
-      </c>
-      <c r="M19">
-        <v>47260.58</v>
-      </c>
-      <c r="N19">
-        <v>24.61</v>
-      </c>
-      <c r="O19">
-        <v>58</v>
-      </c>
-      <c r="P19">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>1100</v>
       </c>
       <c r="B20">
         <v>259.2</v>
       </c>
-      <c r="C20" s="2">
-        <f t="shared" si="0"/>
-        <v>185.14285714285714</v>
-      </c>
-      <c r="D20" t="s">
-        <v>17</v>
+      <c r="C20" t="s">
+        <v>16</v>
+      </c>
+      <c r="D20">
+        <v>192783.5</v>
       </c>
       <c r="E20">
-        <v>192783.5</v>
+        <v>392886.42</v>
       </c>
       <c r="F20">
-        <v>391640.86</v>
+        <v>195909.92</v>
       </c>
       <c r="G20">
-        <v>194681.06</v>
+        <v>196976.5</v>
       </c>
       <c r="H20">
-        <v>196959.8</v>
+        <v>280.01</v>
       </c>
       <c r="I20">
-        <v>271.91000000000003</v>
+        <v>100</v>
       </c>
       <c r="J20">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="K20">
-        <v>50</v>
+        <v>52158.15</v>
       </c>
       <c r="L20">
-        <v>51829.3</v>
+        <v>47685.14</v>
       </c>
       <c r="M20">
-        <v>47381.1</v>
+        <v>22.58</v>
       </c>
       <c r="N20">
-        <v>22.43</v>
+        <v>32</v>
       </c>
       <c r="O20">
-        <v>32</v>
-      </c>
-      <c r="P20">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>1200</v>
       </c>
       <c r="B21">
         <v>259.2</v>
       </c>
-      <c r="C21" s="2">
-        <f t="shared" si="0"/>
-        <v>185.14285714285714</v>
-      </c>
-      <c r="D21" t="s">
-        <v>17</v>
+      <c r="C21" t="s">
+        <v>16</v>
+      </c>
+      <c r="D21">
+        <v>192783.5</v>
       </c>
       <c r="E21">
-        <v>192783.5</v>
+        <v>392886.42</v>
       </c>
       <c r="F21">
-        <v>391640.86</v>
+        <v>195764.08</v>
       </c>
       <c r="G21">
-        <v>194535.23</v>
+        <v>197122.34</v>
       </c>
       <c r="H21">
-        <v>197105.63</v>
+        <v>193.61</v>
       </c>
       <c r="I21">
-        <v>185.51</v>
+        <v>100</v>
       </c>
       <c r="J21">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="K21">
-        <v>50</v>
+        <v>52303.99</v>
       </c>
       <c r="L21">
-        <v>51975.14</v>
+        <v>47771.54</v>
       </c>
       <c r="M21">
-        <v>47467.5</v>
+        <v>20.73</v>
       </c>
       <c r="N21">
-        <v>20.6</v>
+        <v>30</v>
       </c>
       <c r="O21">
-        <v>30</v>
-      </c>
-      <c r="P21">
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>1300</v>
       </c>
       <c r="B22">
         <v>259.2</v>
       </c>
-      <c r="C22" s="2">
-        <f t="shared" si="0"/>
-        <v>185.14285714285714</v>
-      </c>
-      <c r="D22" t="s">
-        <v>17</v>
+      <c r="C22" t="s">
+        <v>16</v>
+      </c>
+      <c r="D22">
+        <v>192783.5</v>
       </c>
       <c r="E22">
-        <v>192783.5</v>
+        <v>392886.42</v>
       </c>
       <c r="F22">
-        <v>391640.86</v>
+        <v>195618.25</v>
       </c>
       <c r="G22">
-        <v>194389.39</v>
+        <v>197268.17</v>
       </c>
       <c r="H22">
-        <v>197251.47</v>
+        <v>107.21</v>
       </c>
       <c r="I22">
-        <v>99.11</v>
+        <v>100</v>
       </c>
       <c r="J22">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="K22">
-        <v>50</v>
+        <v>52449.82</v>
       </c>
       <c r="L22">
-        <v>52120.97</v>
+        <v>47857.94</v>
       </c>
       <c r="M22">
-        <v>47553.9</v>
+        <v>19.170000000000002</v>
       </c>
       <c r="N22">
-        <v>19.05</v>
+        <v>28</v>
       </c>
       <c r="O22">
-        <v>28</v>
-      </c>
-      <c r="P22">
         <v>14</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>1400</v>
       </c>
       <c r="B23">
         <v>259.2</v>
       </c>
-      <c r="C23" s="2">
-        <f t="shared" si="0"/>
-        <v>185.14285714285714</v>
-      </c>
-      <c r="D23" t="s">
-        <v>17</v>
+      <c r="C23" t="s">
+        <v>16</v>
+      </c>
+      <c r="D23">
+        <v>192783.5</v>
       </c>
       <c r="E23">
-        <v>192783.5</v>
+        <v>392886.42</v>
       </c>
       <c r="F23">
-        <v>391640.86</v>
+        <v>195472.42</v>
       </c>
       <c r="G23">
-        <v>194243.56</v>
+        <v>197414</v>
       </c>
       <c r="H23">
-        <v>197397.3</v>
+        <v>20.81</v>
       </c>
       <c r="I23">
-        <v>12.71</v>
+        <v>100</v>
       </c>
       <c r="J23">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="K23">
-        <v>50</v>
+        <v>52595.65</v>
       </c>
       <c r="L23">
-        <v>52266.8</v>
+        <v>47944.34</v>
       </c>
       <c r="M23">
-        <v>47640.3</v>
+        <v>17.84</v>
       </c>
       <c r="N23">
-        <v>17.72</v>
+        <v>14</v>
       </c>
       <c r="O23">
-        <v>9</v>
-      </c>
-      <c r="P23">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>1500</v>
       </c>
       <c r="B24">
         <v>259.2</v>
       </c>
-      <c r="C24" s="2">
-        <f t="shared" si="0"/>
-        <v>185.14285714285714</v>
-      </c>
-      <c r="D24" t="s">
-        <v>17</v>
+      <c r="C24" t="s">
+        <v>16</v>
+      </c>
+      <c r="D24">
+        <v>192783.5</v>
       </c>
       <c r="E24">
-        <v>192783.5</v>
+        <v>392886.42</v>
       </c>
       <c r="F24">
-        <v>391640.86</v>
+        <v>195397.76000000001</v>
       </c>
       <c r="G24">
-        <v>194177.69</v>
+        <v>197488.66</v>
       </c>
       <c r="H24">
-        <v>197463.17</v>
+        <v>0</v>
       </c>
       <c r="I24">
+        <v>100</v>
+      </c>
+      <c r="J24">
+        <v>50</v>
+      </c>
+      <c r="K24">
+        <v>52670.32</v>
+      </c>
+      <c r="L24">
+        <v>47965.15</v>
+      </c>
+      <c r="M24">
+        <v>16.649999999999999</v>
+      </c>
+      <c r="N24">
         <v>0</v>
-      </c>
-      <c r="J24">
-        <v>100</v>
-      </c>
-      <c r="K24">
-        <v>50</v>
-      </c>
-      <c r="L24">
-        <v>52332.67</v>
-      </c>
-      <c r="M24">
-        <v>47653</v>
-      </c>
-      <c r="N24">
-        <v>16.55</v>
       </c>
       <c r="O24">
         <v>0</v>
       </c>
-      <c r="P24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>100</v>
       </c>
       <c r="B25">
         <v>259.2</v>
       </c>
-      <c r="C25" s="2">
-        <f t="shared" si="0"/>
-        <v>185.14285714285714</v>
-      </c>
-      <c r="D25" t="s">
-        <v>18</v>
+      <c r="C25" t="s">
+        <v>17</v>
+      </c>
+      <c r="D25">
+        <v>98582.5</v>
       </c>
       <c r="E25">
-        <v>98582.5</v>
+        <v>392886.42</v>
       </c>
       <c r="F25">
-        <v>391640.86</v>
+        <v>294489.53000000003</v>
       </c>
       <c r="G25">
-        <v>293183.42</v>
+        <v>98396.89</v>
       </c>
       <c r="H25">
-        <v>98457.44</v>
+        <v>1883.54</v>
       </c>
       <c r="I25">
-        <v>1815.02</v>
+        <v>98</v>
       </c>
       <c r="J25">
-        <v>98</v>
+        <v>25</v>
       </c>
       <c r="K25">
-        <v>25</v>
+        <v>21750.87</v>
       </c>
       <c r="L25">
-        <v>21641.25</v>
+        <v>20052.939999999999</v>
       </c>
       <c r="M25">
-        <v>19951.29</v>
+        <v>104.4</v>
       </c>
       <c r="N25">
-        <v>103.88</v>
+        <v>844</v>
       </c>
       <c r="O25">
-        <v>812</v>
-      </c>
-      <c r="P25">
         <v>20</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>200</v>
       </c>
       <c r="B26">
         <v>259.2</v>
       </c>
-      <c r="C26" s="2">
-        <f t="shared" si="0"/>
-        <v>185.14285714285714</v>
-      </c>
-      <c r="D26" t="s">
+      <c r="C26" t="s">
+        <v>17</v>
+      </c>
+      <c r="D26">
+        <v>98582.5</v>
+      </c>
+      <c r="E26">
+        <v>392886.42</v>
+      </c>
+      <c r="F26">
+        <v>292754.5</v>
+      </c>
+      <c r="G26">
+        <v>100131.91</v>
+      </c>
+      <c r="H26">
+        <v>332.54</v>
+      </c>
+      <c r="I26">
+        <v>100</v>
+      </c>
+      <c r="J26">
+        <v>25</v>
+      </c>
+      <c r="K26">
+        <v>23485.9</v>
+      </c>
+      <c r="L26">
+        <v>21603.94</v>
+      </c>
+      <c r="M26">
+        <v>56.26</v>
+      </c>
+      <c r="N26">
+        <v>108</v>
+      </c>
+      <c r="O26">
         <v>18</v>
       </c>
-      <c r="E26">
-        <v>98582.5</v>
-      </c>
-      <c r="F26">
-        <v>391640.86</v>
-      </c>
-      <c r="G26">
-        <v>291508.55</v>
-      </c>
-      <c r="H26">
-        <v>100132.31</v>
-      </c>
-      <c r="I26">
-        <v>319.45999999999998</v>
-      </c>
-      <c r="J26">
-        <v>100</v>
-      </c>
-      <c r="K26">
-        <v>26</v>
-      </c>
-      <c r="L26">
-        <v>23316.12</v>
-      </c>
-      <c r="M26">
-        <v>21446.85</v>
-      </c>
-      <c r="N26">
-        <v>55.85</v>
-      </c>
-      <c r="O26">
-        <v>103</v>
-      </c>
-      <c r="P26">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>300</v>
       </c>
       <c r="B27">
         <v>259.2</v>
       </c>
-      <c r="C27" s="2">
-        <f t="shared" si="0"/>
-        <v>185.14285714285714</v>
-      </c>
-      <c r="D27" t="s">
-        <v>18</v>
+      <c r="C27" t="s">
+        <v>17</v>
+      </c>
+      <c r="D27">
+        <v>98582.5</v>
       </c>
       <c r="E27">
-        <v>98582.5</v>
+        <v>392886.42</v>
       </c>
       <c r="F27">
-        <v>391640.86</v>
+        <v>292489.09999999998</v>
       </c>
       <c r="G27">
-        <v>291256.87</v>
+        <v>100397.32</v>
       </c>
       <c r="H27">
-        <v>100383.99</v>
+        <v>135.94999999999999</v>
       </c>
       <c r="I27">
-        <v>135.51</v>
+        <v>100</v>
       </c>
       <c r="J27">
-        <v>100</v>
+        <v>26</v>
       </c>
       <c r="K27">
-        <v>26</v>
+        <v>23751.3</v>
       </c>
       <c r="L27">
-        <v>23567.8</v>
+        <v>21800.53</v>
       </c>
       <c r="M27">
-        <v>21630.79</v>
+        <v>37.85</v>
       </c>
       <c r="N27">
-        <v>37.549999999999997</v>
+        <v>31</v>
       </c>
       <c r="O27">
-        <v>31</v>
-      </c>
-      <c r="P27">
         <v>15</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>400</v>
       </c>
       <c r="B28">
         <v>259.2</v>
       </c>
-      <c r="C28" s="2">
-        <f t="shared" si="0"/>
-        <v>185.14285714285714</v>
-      </c>
-      <c r="D28" t="s">
-        <v>18</v>
+      <c r="C28" t="s">
+        <v>17</v>
+      </c>
+      <c r="D28">
+        <v>98582.5</v>
       </c>
       <c r="E28">
-        <v>98582.5</v>
+        <v>392886.42</v>
       </c>
       <c r="F28">
-        <v>391640.86</v>
+        <v>292343.27</v>
       </c>
       <c r="G28">
-        <v>291111.03999999998</v>
+        <v>100543.15</v>
       </c>
       <c r="H28">
-        <v>100529.82</v>
+        <v>49.55</v>
       </c>
       <c r="I28">
-        <v>49.11</v>
+        <v>100</v>
       </c>
       <c r="J28">
-        <v>100</v>
+        <v>26</v>
       </c>
       <c r="K28">
-        <v>26</v>
+        <v>23897.13</v>
       </c>
       <c r="L28">
-        <v>23713.63</v>
+        <v>21886.93</v>
       </c>
       <c r="M28">
-        <v>21717.19</v>
+        <v>28.5</v>
       </c>
       <c r="N28">
-        <v>28.28</v>
+        <v>27</v>
       </c>
       <c r="O28">
-        <v>27</v>
-      </c>
-      <c r="P28">
         <v>13</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>500</v>
       </c>
       <c r="B29">
         <v>259.2</v>
       </c>
-      <c r="C29" s="2">
-        <f t="shared" si="0"/>
-        <v>185.14285714285714</v>
-      </c>
-      <c r="D29" t="s">
-        <v>18</v>
+      <c r="C29" t="s">
+        <v>17</v>
+      </c>
+      <c r="D29">
+        <v>98582.5</v>
       </c>
       <c r="E29">
-        <v>98582.5</v>
+        <v>392886.42</v>
       </c>
       <c r="F29">
-        <v>391640.86</v>
+        <v>292237.42</v>
       </c>
       <c r="G29">
-        <v>291005.65999999997</v>
+        <v>100649</v>
       </c>
       <c r="H29">
-        <v>100635.2</v>
+        <v>0</v>
       </c>
       <c r="I29">
+        <v>100</v>
+      </c>
+      <c r="J29">
+        <v>26</v>
+      </c>
+      <c r="K29">
+        <v>24002.98</v>
+      </c>
+      <c r="L29">
+        <v>21936.48</v>
+      </c>
+      <c r="M29">
+        <v>22.85</v>
+      </c>
+      <c r="N29">
         <v>0</v>
-      </c>
-      <c r="J29">
-        <v>100</v>
-      </c>
-      <c r="K29">
-        <v>26</v>
-      </c>
-      <c r="L29">
-        <v>23819</v>
-      </c>
-      <c r="M29">
-        <v>21766.31</v>
-      </c>
-      <c r="N29">
-        <v>22.67</v>
       </c>
       <c r="O29">
         <v>0</v>
       </c>
-      <c r="P29">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>100</v>
       </c>
       <c r="B30">
-        <v>194</v>
-      </c>
-      <c r="C30" s="2">
-        <f t="shared" si="0"/>
-        <v>138.57142857142858</v>
-      </c>
-      <c r="D30" t="s">
-        <v>18</v>
+        <v>194.4</v>
+      </c>
+      <c r="C30" t="s">
+        <v>17</v>
+      </c>
+      <c r="D30">
+        <v>98582.5</v>
       </c>
       <c r="E30">
-        <v>98582.5</v>
+        <v>294664.96000000002</v>
       </c>
       <c r="F30">
-        <v>293730.77</v>
+        <v>197596.82</v>
       </c>
       <c r="G30">
-        <v>196584.68</v>
+        <v>97068.14</v>
       </c>
       <c r="H30">
-        <v>97146.09</v>
+        <v>3321.05</v>
       </c>
       <c r="I30">
-        <v>3236.24</v>
+        <v>97</v>
       </c>
       <c r="J30">
-        <v>97</v>
+        <v>33</v>
       </c>
       <c r="K30">
-        <v>33</v>
+        <v>23208.720000000001</v>
       </c>
       <c r="L30">
-        <v>23115.26</v>
+        <v>21402.04</v>
       </c>
       <c r="M30">
-        <v>21315.439999999999</v>
+        <v>111.4</v>
       </c>
       <c r="N30">
-        <v>110.95</v>
+        <v>1469</v>
       </c>
       <c r="O30">
-        <v>1428</v>
-      </c>
-      <c r="P30">
         <v>23</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>200</v>
       </c>
       <c r="B31">
-        <v>194</v>
-      </c>
-      <c r="C31" s="2">
-        <f t="shared" si="0"/>
-        <v>138.57142857142858</v>
-      </c>
-      <c r="D31" t="s">
+        <v>194.4</v>
+      </c>
+      <c r="C31" t="s">
+        <v>17</v>
+      </c>
+      <c r="D31">
+        <v>98582.5</v>
+      </c>
+      <c r="E31">
+        <v>294664.96000000002</v>
+      </c>
+      <c r="F31">
+        <v>194605.62</v>
+      </c>
+      <c r="G31">
+        <v>100059.34</v>
+      </c>
+      <c r="H31">
+        <v>612.35</v>
+      </c>
+      <c r="I31">
+        <v>99</v>
+      </c>
+      <c r="J31">
+        <v>34</v>
+      </c>
+      <c r="K31">
+        <v>26199.93</v>
+      </c>
+      <c r="L31">
+        <v>24110.73</v>
+      </c>
+      <c r="M31">
+        <v>62.79</v>
+      </c>
+      <c r="N31">
+        <v>188</v>
+      </c>
+      <c r="O31">
         <v>18</v>
       </c>
-      <c r="E31">
-        <v>98582.5</v>
-      </c>
-      <c r="F31">
-        <v>293730.77</v>
-      </c>
-      <c r="G31">
-        <v>193661.91</v>
-      </c>
-      <c r="H31">
-        <v>100068.87</v>
-      </c>
-      <c r="I31">
-        <v>590.61</v>
-      </c>
-      <c r="J31">
-        <v>99</v>
-      </c>
-      <c r="K31">
-        <v>34</v>
-      </c>
-      <c r="L31">
-        <v>26038.04</v>
-      </c>
-      <c r="M31">
-        <v>23961.06</v>
-      </c>
-      <c r="N31">
-        <v>62.4</v>
-      </c>
-      <c r="O31">
-        <v>180</v>
-      </c>
-      <c r="P31">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>300</v>
       </c>
       <c r="B32">
-        <v>194</v>
-      </c>
-      <c r="C32" s="2">
-        <f t="shared" si="0"/>
-        <v>138.57142857142858</v>
-      </c>
-      <c r="D32" t="s">
-        <v>18</v>
+        <v>194.4</v>
+      </c>
+      <c r="C32" t="s">
+        <v>17</v>
+      </c>
+      <c r="D32">
+        <v>98582.5</v>
       </c>
       <c r="E32">
-        <v>98582.5</v>
+        <v>294664.96000000002</v>
       </c>
       <c r="F32">
-        <v>293730.77</v>
+        <v>194115.9</v>
       </c>
       <c r="G32">
-        <v>193187.08</v>
+        <v>100549.06</v>
       </c>
       <c r="H32">
-        <v>100543.69</v>
+        <v>209.03</v>
       </c>
       <c r="I32">
-        <v>201.01</v>
+        <v>100</v>
       </c>
       <c r="J32">
-        <v>100</v>
+        <v>34</v>
       </c>
       <c r="K32">
-        <v>34</v>
+        <v>26689.65</v>
       </c>
       <c r="L32">
-        <v>26512.86</v>
+        <v>24514.05</v>
       </c>
       <c r="M32">
-        <v>24350.66</v>
+        <v>42.56</v>
       </c>
       <c r="N32">
-        <v>42.28</v>
+        <v>65</v>
       </c>
       <c r="O32">
-        <v>60</v>
-      </c>
-      <c r="P32">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>400</v>
       </c>
       <c r="B33">
-        <v>194</v>
-      </c>
-      <c r="C33" s="2">
-        <f t="shared" si="0"/>
-        <v>138.57142857142858</v>
-      </c>
-      <c r="D33" t="s">
-        <v>18</v>
+        <v>194.4</v>
+      </c>
+      <c r="C33" t="s">
+        <v>17</v>
+      </c>
+      <c r="D33">
+        <v>98582.5</v>
       </c>
       <c r="E33">
-        <v>98582.5</v>
+        <v>294664.96000000002</v>
       </c>
       <c r="F33">
-        <v>293730.77</v>
+        <v>193919.97</v>
       </c>
       <c r="G33">
-        <v>192998.63</v>
+        <v>100744.99</v>
       </c>
       <c r="H33">
-        <v>100732.14</v>
+        <v>76.459999999999994</v>
       </c>
       <c r="I33">
-        <v>75.33</v>
+        <v>100</v>
       </c>
       <c r="J33">
-        <v>100</v>
+        <v>34</v>
       </c>
       <c r="K33">
-        <v>34</v>
+        <v>26885.57</v>
       </c>
       <c r="L33">
-        <v>26701.31</v>
+        <v>24646.62</v>
       </c>
       <c r="M33">
-        <v>24476.34</v>
+        <v>32.090000000000003</v>
       </c>
       <c r="N33">
-        <v>31.87</v>
+        <v>28</v>
       </c>
       <c r="O33">
-        <v>28</v>
-      </c>
-      <c r="P33">
         <v>14</v>
       </c>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>500</v>
       </c>
       <c r="B34">
-        <v>194</v>
-      </c>
-      <c r="C34" s="2">
-        <f t="shared" si="0"/>
-        <v>138.57142857142858</v>
-      </c>
-      <c r="D34" t="s">
-        <v>18</v>
+        <v>194.4</v>
+      </c>
+      <c r="C34" t="s">
+        <v>17</v>
+      </c>
+      <c r="D34">
+        <v>98582.5</v>
       </c>
       <c r="E34">
-        <v>98582.5</v>
+        <v>294664.96000000002</v>
       </c>
       <c r="F34">
-        <v>293730.77</v>
+        <v>193784.92</v>
       </c>
       <c r="G34">
-        <v>192864.81</v>
+        <v>100880.04</v>
       </c>
       <c r="H34">
-        <v>100865.96</v>
+        <v>0</v>
       </c>
       <c r="I34">
+        <v>100</v>
+      </c>
+      <c r="J34">
+        <v>34</v>
+      </c>
+      <c r="K34">
+        <v>27020.62</v>
+      </c>
+      <c r="L34">
+        <v>24723.08</v>
+      </c>
+      <c r="M34">
+        <v>25.75</v>
+      </c>
+      <c r="N34">
         <v>0</v>
-      </c>
-      <c r="J34">
-        <v>100</v>
-      </c>
-      <c r="K34">
-        <v>34</v>
-      </c>
-      <c r="L34">
-        <v>26835.14</v>
-      </c>
-      <c r="M34">
-        <v>24551.67</v>
-      </c>
-      <c r="N34">
-        <v>25.57</v>
       </c>
       <c r="O34">
         <v>0</v>
       </c>
-      <c r="P34">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>100</v>
       </c>
       <c r="B35">
-        <v>194</v>
-      </c>
-      <c r="C35" s="2">
-        <f t="shared" si="0"/>
-        <v>138.57142857142858</v>
-      </c>
-      <c r="D35" t="s">
-        <v>16</v>
+        <v>194.4</v>
+      </c>
+      <c r="C35" t="s">
+        <v>15</v>
+      </c>
+      <c r="D35">
+        <v>135543.5</v>
       </c>
       <c r="E35">
-        <v>135543.5</v>
+        <v>294664.96000000002</v>
       </c>
       <c r="F35">
-        <v>293730.77</v>
+        <v>170465.94</v>
       </c>
       <c r="G35">
-        <v>169353.57</v>
+        <v>124199.03</v>
       </c>
       <c r="H35">
-        <v>124377.2</v>
+        <v>13465.73</v>
       </c>
       <c r="I35">
-        <v>13283.47</v>
+        <v>90</v>
       </c>
       <c r="J35">
-        <v>90</v>
+        <v>42</v>
       </c>
       <c r="K35">
-        <v>42</v>
+        <v>27546.65</v>
       </c>
       <c r="L35">
-        <v>27494.5</v>
+        <v>25425.4</v>
       </c>
       <c r="M35">
-        <v>25377.34</v>
+        <v>132.22</v>
       </c>
       <c r="N35">
-        <v>131.97</v>
+        <v>4225</v>
       </c>
       <c r="O35">
-        <v>4182</v>
-      </c>
-      <c r="P35">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.2">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>200</v>
       </c>
       <c r="B36">
-        <v>194</v>
-      </c>
-      <c r="C36" s="2">
-        <f t="shared" si="0"/>
-        <v>138.57142857142858</v>
-      </c>
-      <c r="D36" t="s">
-        <v>16</v>
+        <v>194.4</v>
+      </c>
+      <c r="C36" t="s">
+        <v>15</v>
+      </c>
+      <c r="D36">
+        <v>135543.5</v>
       </c>
       <c r="E36">
-        <v>135543.5</v>
+        <v>294664.96000000002</v>
       </c>
       <c r="F36">
-        <v>293730.77</v>
+        <v>160487.24</v>
       </c>
       <c r="G36">
-        <v>159463.67000000001</v>
+        <v>134177.73000000001</v>
       </c>
       <c r="H36">
-        <v>134267.1</v>
+        <v>4273.88</v>
       </c>
       <c r="I36">
-        <v>4174.32</v>
+        <v>97</v>
       </c>
       <c r="J36">
-        <v>97</v>
+        <v>46</v>
       </c>
       <c r="K36">
-        <v>46</v>
+        <v>37525.35</v>
       </c>
       <c r="L36">
-        <v>37384.410000000003</v>
+        <v>34617.25</v>
       </c>
       <c r="M36">
-        <v>34486.49</v>
+        <v>90.06</v>
       </c>
       <c r="N36">
-        <v>89.72</v>
+        <v>1194</v>
       </c>
       <c r="O36">
-        <v>1162</v>
-      </c>
-      <c r="P36">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.2">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>300</v>
       </c>
       <c r="B37">
-        <v>194</v>
-      </c>
-      <c r="C37" s="2">
-        <f t="shared" si="0"/>
-        <v>138.57142857142858</v>
-      </c>
-      <c r="D37" t="s">
-        <v>16</v>
+        <v>194.4</v>
+      </c>
+      <c r="C37" t="s">
+        <v>15</v>
+      </c>
+      <c r="D37">
+        <v>135543.5</v>
       </c>
       <c r="E37">
-        <v>135543.5</v>
+        <v>294664.96000000002</v>
       </c>
       <c r="F37">
-        <v>293730.77</v>
+        <v>158131.73000000001</v>
       </c>
       <c r="G37">
-        <v>157148.96</v>
+        <v>136533.23000000001</v>
       </c>
       <c r="H37">
-        <v>136581.82</v>
+        <v>2151.04</v>
       </c>
       <c r="I37">
-        <v>2089.08</v>
+        <v>98</v>
       </c>
       <c r="J37">
-        <v>98</v>
+        <v>46</v>
       </c>
       <c r="K37">
-        <v>46</v>
+        <v>39880.86</v>
       </c>
       <c r="L37">
-        <v>39699.120000000003</v>
+        <v>36740.080000000002</v>
       </c>
       <c r="M37">
-        <v>36571.730000000003</v>
+        <v>63.78</v>
       </c>
       <c r="N37">
-        <v>63.49</v>
+        <v>534</v>
       </c>
       <c r="O37">
-        <v>516</v>
-      </c>
-      <c r="P37">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.2">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>400</v>
       </c>
       <c r="B38">
-        <v>194</v>
-      </c>
-      <c r="C38" s="2">
-        <f t="shared" si="0"/>
-        <v>138.57142857142858</v>
-      </c>
-      <c r="D38" t="s">
-        <v>16</v>
+        <v>194.4</v>
+      </c>
+      <c r="C38" t="s">
+        <v>15</v>
+      </c>
+      <c r="D38">
+        <v>135543.5</v>
       </c>
       <c r="E38">
-        <v>135543.5</v>
+        <v>294664.96000000002</v>
       </c>
       <c r="F38">
-        <v>293730.77</v>
+        <v>156859.29</v>
       </c>
       <c r="G38">
-        <v>155895.35999999999</v>
+        <v>137805.67000000001</v>
       </c>
       <c r="H38">
-        <v>137835.41</v>
+        <v>1026.3599999999999</v>
       </c>
       <c r="I38">
-        <v>981.76</v>
+        <v>99</v>
       </c>
       <c r="J38">
-        <v>99</v>
+        <v>47</v>
       </c>
       <c r="K38">
-        <v>47</v>
+        <v>41153.300000000003</v>
       </c>
       <c r="L38">
-        <v>40952.720000000001</v>
+        <v>37864.769999999997</v>
       </c>
       <c r="M38">
-        <v>37679.040000000001</v>
+        <v>49.3</v>
       </c>
       <c r="N38">
-        <v>49.06</v>
+        <v>222</v>
       </c>
       <c r="O38">
-        <v>211</v>
-      </c>
-      <c r="P38">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>500</v>
       </c>
       <c r="B39">
-        <v>194</v>
-      </c>
-      <c r="C39" s="2">
-        <f t="shared" si="0"/>
-        <v>138.57142857142858</v>
-      </c>
-      <c r="D39" t="s">
-        <v>16</v>
+        <v>194.4</v>
+      </c>
+      <c r="C39" t="s">
+        <v>15</v>
+      </c>
+      <c r="D39">
+        <v>135543.5</v>
       </c>
       <c r="E39">
-        <v>135543.5</v>
+        <v>294664.96000000002</v>
       </c>
       <c r="F39">
-        <v>293730.77</v>
+        <v>156218.21</v>
       </c>
       <c r="G39">
-        <v>155274.66</v>
+        <v>138446.76</v>
       </c>
       <c r="H39">
-        <v>138456.10999999999</v>
+        <v>483.54</v>
       </c>
       <c r="I39">
-        <v>457.73</v>
+        <v>100</v>
       </c>
       <c r="J39">
-        <v>100</v>
+        <v>47</v>
       </c>
       <c r="K39">
-        <v>47</v>
+        <v>41794.379999999997</v>
       </c>
       <c r="L39">
-        <v>41573.42</v>
+        <v>38407.589999999997</v>
       </c>
       <c r="M39">
-        <v>38203.08</v>
+        <v>40.01</v>
       </c>
       <c r="N39">
-        <v>39.79</v>
+        <v>103</v>
       </c>
       <c r="O39">
-        <v>96</v>
-      </c>
-      <c r="P39">
         <v>18</v>
       </c>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>600</v>
       </c>
       <c r="B40">
-        <v>194</v>
-      </c>
-      <c r="C40" s="2">
-        <f t="shared" si="0"/>
-        <v>138.57142857142858</v>
-      </c>
-      <c r="D40" t="s">
-        <v>16</v>
+        <v>194.4</v>
+      </c>
+      <c r="C40" t="s">
+        <v>15</v>
+      </c>
+      <c r="D40">
+        <v>135543.5</v>
       </c>
       <c r="E40">
-        <v>135543.5</v>
+        <v>294664.96000000002</v>
       </c>
       <c r="F40">
-        <v>293730.77</v>
+        <v>155936.12</v>
       </c>
       <c r="G40">
-        <v>155016.04</v>
+        <v>138728.84</v>
       </c>
       <c r="H40">
-        <v>138714.74</v>
+        <v>271.57</v>
       </c>
       <c r="I40">
-        <v>267.38</v>
+        <v>100</v>
       </c>
       <c r="J40">
-        <v>100</v>
+        <v>47</v>
       </c>
       <c r="K40">
-        <v>47</v>
+        <v>42076.47</v>
       </c>
       <c r="L40">
-        <v>41832.04</v>
+        <v>38619.56</v>
       </c>
       <c r="M40">
-        <v>38393.43</v>
+        <v>33.520000000000003</v>
       </c>
       <c r="N40">
-        <v>33.33</v>
+        <v>34</v>
       </c>
       <c r="O40">
-        <v>34</v>
-      </c>
-      <c r="P40">
         <v>17</v>
       </c>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>700</v>
       </c>
       <c r="B41">
-        <v>194</v>
-      </c>
-      <c r="C41" s="2">
-        <f t="shared" si="0"/>
-        <v>138.57142857142858</v>
-      </c>
-      <c r="D41" t="s">
-        <v>16</v>
+        <v>194.4</v>
+      </c>
+      <c r="C41" t="s">
+        <v>15</v>
+      </c>
+      <c r="D41">
+        <v>135543.5</v>
       </c>
       <c r="E41">
-        <v>135543.5</v>
+        <v>294664.96000000002</v>
       </c>
       <c r="F41">
-        <v>293730.77</v>
+        <v>155790.28</v>
       </c>
       <c r="G41">
-        <v>154870.21</v>
+        <v>138874.68</v>
       </c>
       <c r="H41">
-        <v>138860.57</v>
+        <v>185.17</v>
       </c>
       <c r="I41">
-        <v>180.98</v>
+        <v>100</v>
       </c>
       <c r="J41">
-        <v>100</v>
+        <v>47</v>
       </c>
       <c r="K41">
-        <v>47</v>
+        <v>42222.31</v>
       </c>
       <c r="L41">
-        <v>41977.87</v>
+        <v>38705.96</v>
       </c>
       <c r="M41">
-        <v>38479.83</v>
+        <v>28.8</v>
       </c>
       <c r="N41">
-        <v>28.63</v>
+        <v>31</v>
       </c>
       <c r="O41">
-        <v>31</v>
-      </c>
-      <c r="P41">
         <v>15</v>
       </c>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>800</v>
       </c>
       <c r="B42">
-        <v>194</v>
-      </c>
-      <c r="C42" s="2">
-        <f t="shared" si="0"/>
-        <v>138.57142857142858</v>
-      </c>
-      <c r="D42" t="s">
-        <v>16</v>
+        <v>194.4</v>
+      </c>
+      <c r="C42" t="s">
+        <v>15</v>
+      </c>
+      <c r="D42">
+        <v>135543.5</v>
       </c>
       <c r="E42">
-        <v>135543.5</v>
+        <v>294664.96000000002</v>
       </c>
       <c r="F42">
-        <v>293730.77</v>
+        <v>155644.45000000001</v>
       </c>
       <c r="G42">
-        <v>154724.37</v>
+        <v>139020.51</v>
       </c>
       <c r="H42">
-        <v>139006.39999999999</v>
+        <v>98.77</v>
       </c>
       <c r="I42">
-        <v>94.58</v>
+        <v>100</v>
       </c>
       <c r="J42">
-        <v>100</v>
+        <v>47</v>
       </c>
       <c r="K42">
-        <v>47</v>
+        <v>42368.14</v>
       </c>
       <c r="L42">
-        <v>42123.71</v>
+        <v>38792.36</v>
       </c>
       <c r="M42">
-        <v>38566.230000000003</v>
+        <v>25.26</v>
       </c>
       <c r="N42">
-        <v>25.11</v>
+        <v>28</v>
       </c>
       <c r="O42">
-        <v>28</v>
-      </c>
-      <c r="P42">
         <v>14</v>
       </c>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>900</v>
       </c>
       <c r="B43">
-        <v>194</v>
-      </c>
-      <c r="C43" s="2">
-        <f t="shared" si="0"/>
-        <v>138.57142857142858</v>
-      </c>
-      <c r="D43" t="s">
-        <v>16</v>
+        <v>194.4</v>
+      </c>
+      <c r="C43" t="s">
+        <v>15</v>
+      </c>
+      <c r="D43">
+        <v>135543.5</v>
       </c>
       <c r="E43">
-        <v>135543.5</v>
+        <v>294664.96000000002</v>
       </c>
       <c r="F43">
-        <v>293730.77</v>
+        <v>155498.62</v>
       </c>
       <c r="G43">
-        <v>154578.54</v>
+        <v>139166.34</v>
       </c>
       <c r="H43">
-        <v>139152.24</v>
+        <v>12.37</v>
       </c>
       <c r="I43">
-        <v>8.18</v>
+        <v>100</v>
       </c>
       <c r="J43">
-        <v>100</v>
+        <v>47</v>
       </c>
       <c r="K43">
-        <v>47</v>
+        <v>42513.97</v>
       </c>
       <c r="L43">
-        <v>42269.54</v>
+        <v>38878.76</v>
       </c>
       <c r="M43">
-        <v>38652.629999999997</v>
+        <v>22.5</v>
       </c>
       <c r="N43">
-        <v>22.37</v>
+        <v>9</v>
       </c>
       <c r="O43">
-        <v>6</v>
-      </c>
-      <c r="P43">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>1000</v>
       </c>
       <c r="B44">
-        <v>194</v>
-      </c>
-      <c r="C44" s="2">
-        <f t="shared" si="0"/>
-        <v>138.57142857142858</v>
-      </c>
-      <c r="D44" t="s">
-        <v>16</v>
+        <v>194.4</v>
+      </c>
+      <c r="C44" t="s">
+        <v>15</v>
+      </c>
+      <c r="D44">
+        <v>135543.5</v>
       </c>
       <c r="E44">
-        <v>135543.5</v>
+        <v>294664.96000000002</v>
       </c>
       <c r="F44">
-        <v>293730.77</v>
+        <v>155433.10999999999</v>
       </c>
       <c r="G44">
-        <v>154517.57999999999</v>
+        <v>139231.85</v>
       </c>
       <c r="H44">
-        <v>139213.19</v>
+        <v>0</v>
       </c>
       <c r="I44">
+        <v>100</v>
+      </c>
+      <c r="J44">
+        <v>47</v>
+      </c>
+      <c r="K44">
+        <v>42579.48</v>
+      </c>
+      <c r="L44">
+        <v>38891.129999999997</v>
+      </c>
+      <c r="M44">
+        <v>20.260000000000002</v>
+      </c>
+      <c r="N44">
         <v>0</v>
-      </c>
-      <c r="J44">
-        <v>100</v>
-      </c>
-      <c r="K44">
-        <v>47</v>
-      </c>
-      <c r="L44">
-        <v>42330.5</v>
-      </c>
-      <c r="M44">
-        <v>38660.81</v>
-      </c>
-      <c r="N44">
-        <v>20.14</v>
       </c>
       <c r="O44">
         <v>0</v>
       </c>
-      <c r="P44">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>100</v>
       </c>
       <c r="B45">
-        <v>194</v>
-      </c>
-      <c r="C45" s="2">
-        <f t="shared" si="0"/>
-        <v>138.57142857142858</v>
-      </c>
-      <c r="D45" t="s">
-        <v>17</v>
+        <v>194.4</v>
+      </c>
+      <c r="C45" t="s">
+        <v>16</v>
+      </c>
+      <c r="D45">
+        <v>192783.5</v>
       </c>
       <c r="E45">
-        <v>192783.5</v>
+        <v>294664.96000000002</v>
       </c>
       <c r="F45">
-        <v>293730.77</v>
+        <v>131747.32</v>
       </c>
       <c r="G45">
-        <v>130481.23</v>
+        <v>162917.64000000001</v>
       </c>
       <c r="H45">
-        <v>163249.54</v>
+        <v>32095.53</v>
       </c>
       <c r="I45">
-        <v>31765.18</v>
-      </c>
-      <c r="J45">
-        <v>84</v>
-      </c>
-      <c r="K45" s="1">
-        <v>56</v>
+        <v>83</v>
+      </c>
+      <c r="J45" s="1">
+        <v>55</v>
+      </c>
+      <c r="K45">
+        <v>28929.5</v>
       </c>
       <c r="L45">
-        <v>28949.27</v>
+        <v>26699.83</v>
       </c>
       <c r="M45">
-        <v>26718.05</v>
+        <v>138.86000000000001</v>
       </c>
       <c r="N45">
-        <v>138.96</v>
+        <v>6203</v>
       </c>
       <c r="O45">
-        <v>6141</v>
-      </c>
-      <c r="P45">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>200</v>
       </c>
       <c r="B46">
-        <v>194</v>
-      </c>
-      <c r="C46" s="2">
-        <f t="shared" si="0"/>
-        <v>138.57142857142858</v>
-      </c>
-      <c r="D46" t="s">
-        <v>17</v>
+        <v>194.4</v>
+      </c>
+      <c r="C46" t="s">
+        <v>16</v>
+      </c>
+      <c r="D46">
+        <v>192783.5</v>
       </c>
       <c r="E46">
-        <v>192783.5</v>
+        <v>294664.96000000002</v>
       </c>
       <c r="F46">
-        <v>293730.77</v>
+        <v>117687.48</v>
       </c>
       <c r="G46">
-        <v>116491.04</v>
+        <v>176977.49</v>
       </c>
       <c r="H46">
-        <v>177239.73</v>
+        <v>19099.580000000002</v>
       </c>
       <c r="I46">
-        <v>18833.419999999998</v>
+        <v>90</v>
       </c>
       <c r="J46">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="K46">
-        <v>60</v>
+        <v>42989.34</v>
       </c>
       <c r="L46">
-        <v>42939.46</v>
+        <v>39695.78</v>
       </c>
       <c r="M46">
-        <v>39649.81</v>
+        <v>103.17</v>
       </c>
       <c r="N46">
-        <v>103.05</v>
+        <v>3690</v>
       </c>
       <c r="O46">
-        <v>3642</v>
-      </c>
-      <c r="P46">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>300</v>
       </c>
       <c r="B47">
-        <v>194</v>
-      </c>
-      <c r="C47" s="2">
-        <f t="shared" si="0"/>
-        <v>138.57142857142858</v>
-      </c>
-      <c r="D47" t="s">
-        <v>17</v>
+        <v>194.4</v>
+      </c>
+      <c r="C47" t="s">
+        <v>16</v>
+      </c>
+      <c r="D47">
+        <v>192783.5</v>
       </c>
       <c r="E47">
-        <v>192783.5</v>
+        <v>294664.96000000002</v>
       </c>
       <c r="F47">
-        <v>293730.77</v>
+        <v>111958.17</v>
       </c>
       <c r="G47">
-        <v>110794.76</v>
+        <v>182706.79</v>
       </c>
       <c r="H47">
-        <v>182936.02</v>
+        <v>13845.35</v>
       </c>
       <c r="I47">
-        <v>13613.28</v>
+        <v>93</v>
       </c>
       <c r="J47">
-        <v>93</v>
+        <v>62</v>
       </c>
       <c r="K47">
-        <v>62</v>
+        <v>48718.65</v>
       </c>
       <c r="L47">
-        <v>48635.75</v>
+        <v>44950.01</v>
       </c>
       <c r="M47">
-        <v>44869.95</v>
+        <v>77.95</v>
       </c>
       <c r="N47">
-        <v>77.819999999999993</v>
+        <v>2395</v>
       </c>
       <c r="O47">
-        <v>2363</v>
-      </c>
-      <c r="P47">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>400</v>
       </c>
       <c r="B48">
-        <v>194</v>
-      </c>
-      <c r="C48" s="2">
-        <f t="shared" si="0"/>
-        <v>138.57142857142858</v>
-      </c>
-      <c r="D48" t="s">
-        <v>17</v>
+        <v>194.4</v>
+      </c>
+      <c r="C48" t="s">
+        <v>16</v>
+      </c>
+      <c r="D48">
+        <v>192783.5</v>
       </c>
       <c r="E48">
-        <v>192783.5</v>
+        <v>294664.96000000002</v>
       </c>
       <c r="F48">
-        <v>293730.77</v>
+        <v>108584.58</v>
       </c>
       <c r="G48">
-        <v>107455.36</v>
+        <v>186080.38</v>
       </c>
       <c r="H48">
-        <v>186275.41</v>
+        <v>10784.25</v>
       </c>
       <c r="I48">
-        <v>10583.7</v>
+        <v>94</v>
       </c>
       <c r="J48">
-        <v>95</v>
+        <v>63</v>
       </c>
       <c r="K48">
-        <v>63</v>
+        <v>52092.24</v>
       </c>
       <c r="L48">
-        <v>51975.14</v>
+        <v>48011.1</v>
       </c>
       <c r="M48">
-        <v>47899.53</v>
+        <v>62.51</v>
       </c>
       <c r="N48">
-        <v>62.37</v>
+        <v>1747</v>
       </c>
       <c r="O48">
-        <v>1715</v>
-      </c>
-      <c r="P48">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="49" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>500</v>
       </c>
       <c r="B49">
-        <v>194</v>
-      </c>
-      <c r="C49" s="2">
-        <f t="shared" si="0"/>
-        <v>138.57142857142858</v>
-      </c>
-      <c r="D49" t="s">
-        <v>17</v>
+        <v>194.4</v>
+      </c>
+      <c r="C49" t="s">
+        <v>16</v>
+      </c>
+      <c r="D49">
+        <v>192783.5</v>
       </c>
       <c r="E49">
-        <v>192783.5</v>
+        <v>294664.96000000002</v>
       </c>
       <c r="F49">
-        <v>293730.77</v>
+        <v>106196.5</v>
       </c>
       <c r="G49">
-        <v>105081.1</v>
+        <v>188468.46</v>
       </c>
       <c r="H49">
-        <v>188649.67</v>
+        <v>8631.39</v>
       </c>
       <c r="I49">
-        <v>8443.58</v>
+        <v>96</v>
       </c>
       <c r="J49">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="K49">
-        <v>64</v>
+        <v>54480.32</v>
       </c>
       <c r="L49">
-        <v>54349.4</v>
+        <v>50163.96</v>
       </c>
       <c r="M49">
-        <v>50039.65</v>
+        <v>52.25</v>
       </c>
       <c r="N49">
-        <v>52.12</v>
+        <v>1412</v>
       </c>
       <c r="O49">
-        <v>1389</v>
-      </c>
-      <c r="P49">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="50" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>600</v>
       </c>
       <c r="B50">
-        <v>194</v>
-      </c>
-      <c r="C50" s="2">
-        <f t="shared" si="0"/>
-        <v>138.57142857142858</v>
-      </c>
-      <c r="D50" t="s">
-        <v>17</v>
+        <v>194.4</v>
+      </c>
+      <c r="C50" t="s">
+        <v>16</v>
+      </c>
+      <c r="D50">
+        <v>192783.5</v>
       </c>
       <c r="E50">
-        <v>192783.5</v>
+        <v>294664.96000000002</v>
       </c>
       <c r="F50">
-        <v>293730.77</v>
+        <v>104278.05</v>
       </c>
       <c r="G50">
-        <v>103193.57</v>
+        <v>190386.91</v>
       </c>
       <c r="H50">
-        <v>190537.2</v>
+        <v>6911.36</v>
       </c>
       <c r="I50">
-        <v>6752.03</v>
+        <v>96</v>
       </c>
       <c r="J50">
-        <v>96</v>
+        <v>65</v>
       </c>
       <c r="K50">
-        <v>65</v>
+        <v>56398.77</v>
       </c>
       <c r="L50">
-        <v>56236.94</v>
+        <v>51884</v>
       </c>
       <c r="M50">
-        <v>51731.199999999997</v>
+        <v>45.04</v>
       </c>
       <c r="N50">
-        <v>44.91</v>
+        <v>1091</v>
       </c>
       <c r="O50">
-        <v>1061</v>
-      </c>
-      <c r="P50">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="51" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>700</v>
       </c>
       <c r="B51">
-        <v>194</v>
-      </c>
-      <c r="C51" s="2">
-        <f t="shared" si="0"/>
-        <v>138.57142857142858</v>
-      </c>
-      <c r="D51" t="s">
-        <v>17</v>
+        <v>194.4</v>
+      </c>
+      <c r="C51" t="s">
+        <v>16</v>
+      </c>
+      <c r="D51">
+        <v>192783.5</v>
       </c>
       <c r="E51">
-        <v>192783.5</v>
+        <v>294664.96000000002</v>
       </c>
       <c r="F51">
-        <v>293730.77</v>
+        <v>102761.42</v>
       </c>
       <c r="G51">
-        <v>101690.86</v>
+        <v>191903.54</v>
       </c>
       <c r="H51">
-        <v>192039.91</v>
+        <v>5561.63</v>
       </c>
       <c r="I51">
-        <v>5415.13</v>
+        <v>97</v>
       </c>
       <c r="J51">
-        <v>97</v>
+        <v>65</v>
       </c>
       <c r="K51">
-        <v>65</v>
+        <v>57915.39</v>
       </c>
       <c r="L51">
-        <v>57739.65</v>
+        <v>53233.73</v>
       </c>
       <c r="M51">
-        <v>53068.1</v>
+        <v>39.61</v>
       </c>
       <c r="N51">
-        <v>39.49</v>
+        <v>893</v>
       </c>
       <c r="O51">
-        <v>870</v>
-      </c>
-      <c r="P51">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.2">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="52" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>800</v>
       </c>
       <c r="B52">
-        <v>194</v>
-      </c>
-      <c r="C52" s="2">
-        <f t="shared" si="0"/>
-        <v>138.57142857142858</v>
-      </c>
-      <c r="D52" t="s">
-        <v>17</v>
+        <v>194.4</v>
+      </c>
+      <c r="C52" t="s">
+        <v>16</v>
+      </c>
+      <c r="D52">
+        <v>192783.5</v>
       </c>
       <c r="E52">
-        <v>192783.5</v>
+        <v>294664.96000000002</v>
       </c>
       <c r="F52">
-        <v>293730.77</v>
+        <v>101352.38</v>
       </c>
       <c r="G52">
-        <v>100297.13</v>
+        <v>193312.58</v>
       </c>
       <c r="H52">
-        <v>193433.64</v>
+        <v>4311.05</v>
       </c>
       <c r="I52">
-        <v>4178.67</v>
+        <v>98</v>
       </c>
       <c r="J52">
-        <v>98</v>
+        <v>66</v>
       </c>
       <c r="K52">
-        <v>66</v>
+        <v>59324.44</v>
       </c>
       <c r="L52">
-        <v>59133.37</v>
+        <v>54484.31</v>
       </c>
       <c r="M52">
-        <v>54304.56</v>
+        <v>35.47</v>
       </c>
       <c r="N52">
-        <v>35.35</v>
+        <v>723</v>
       </c>
       <c r="O52">
-        <v>700</v>
-      </c>
-      <c r="P52">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.2">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="53" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>900</v>
       </c>
       <c r="B53">
-        <v>194</v>
-      </c>
-      <c r="C53" s="2">
-        <f t="shared" si="0"/>
-        <v>138.57142857142858</v>
-      </c>
-      <c r="D53" t="s">
-        <v>17</v>
+        <v>194.4</v>
+      </c>
+      <c r="C53" t="s">
+        <v>16</v>
+      </c>
+      <c r="D53">
+        <v>192783.5</v>
       </c>
       <c r="E53">
-        <v>192783.5</v>
+        <v>294664.96000000002</v>
       </c>
       <c r="F53">
-        <v>293730.77</v>
+        <v>100195.47</v>
       </c>
       <c r="G53">
-        <v>99159.8</v>
+        <v>194469.49</v>
       </c>
       <c r="H53">
-        <v>194570.97</v>
+        <v>3292.85</v>
       </c>
       <c r="I53">
-        <v>3178.51</v>
+        <v>98</v>
       </c>
       <c r="J53">
-        <v>98</v>
+        <v>66</v>
       </c>
       <c r="K53">
-        <v>66</v>
+        <v>60481.35</v>
       </c>
       <c r="L53">
-        <v>60270.71</v>
+        <v>55502.51</v>
       </c>
       <c r="M53">
-        <v>55304.72</v>
+        <v>32.119999999999997</v>
       </c>
       <c r="N53">
-        <v>32.01</v>
+        <v>533</v>
       </c>
       <c r="O53">
-        <v>517</v>
-      </c>
-      <c r="P53">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="54" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>1000</v>
       </c>
       <c r="B54">
-        <v>194</v>
-      </c>
-      <c r="C54" s="2">
-        <f t="shared" si="0"/>
-        <v>138.57142857142858</v>
-      </c>
-      <c r="D54" t="s">
-        <v>17</v>
+        <v>194.4</v>
+      </c>
+      <c r="C54" t="s">
+        <v>16</v>
+      </c>
+      <c r="D54">
+        <v>192783.5</v>
       </c>
       <c r="E54">
-        <v>192783.5</v>
+        <v>294664.96000000002</v>
       </c>
       <c r="F54">
-        <v>293730.77</v>
+        <v>99317.759999999995</v>
       </c>
       <c r="G54">
-        <v>98320.77</v>
+        <v>195347.20000000001</v>
       </c>
       <c r="H54">
-        <v>195410.01</v>
+        <v>2531.9499999999998</v>
       </c>
       <c r="I54">
-        <v>2453.2600000000002</v>
+        <v>99</v>
       </c>
       <c r="J54">
-        <v>99</v>
+        <v>66</v>
       </c>
       <c r="K54">
-        <v>67</v>
+        <v>61359.06</v>
       </c>
       <c r="L54">
-        <v>61109.74</v>
+        <v>56263.41</v>
       </c>
       <c r="M54">
-        <v>56029.98</v>
+        <v>29.3</v>
       </c>
       <c r="N54">
-        <v>29.18</v>
+        <v>370</v>
       </c>
       <c r="O54">
-        <v>364</v>
-      </c>
-      <c r="P54">
         <v>20</v>
       </c>
     </row>
-    <row r="55" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>1100</v>
       </c>
       <c r="B55">
-        <v>194</v>
-      </c>
-      <c r="C55" s="2">
-        <f t="shared" si="0"/>
-        <v>138.57142857142858</v>
-      </c>
-      <c r="D55" t="s">
-        <v>17</v>
+        <v>194.4</v>
+      </c>
+      <c r="C55" t="s">
+        <v>16</v>
+      </c>
+      <c r="D55">
+        <v>192783.5</v>
       </c>
       <c r="E55">
-        <v>192783.5</v>
+        <v>294664.96000000002</v>
       </c>
       <c r="F55">
-        <v>293730.77</v>
+        <v>98682.9</v>
       </c>
       <c r="G55">
-        <v>97695.54</v>
+        <v>195982.06</v>
       </c>
       <c r="H55">
-        <v>196035.23</v>
+        <v>1994.86</v>
       </c>
       <c r="I55">
-        <v>1925.05</v>
+        <v>99</v>
       </c>
       <c r="J55">
-        <v>99</v>
+        <v>67</v>
       </c>
       <c r="K55">
-        <v>67</v>
+        <v>61993.919999999998</v>
       </c>
       <c r="L55">
-        <v>61734.96</v>
+        <v>56800.5</v>
       </c>
       <c r="M55">
-        <v>56558.18</v>
+        <v>26.89</v>
       </c>
       <c r="N55">
-        <v>26.78</v>
+        <v>286</v>
       </c>
       <c r="O55">
-        <v>270</v>
-      </c>
-      <c r="P55">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="56" spans="1:16" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="56" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>1200</v>
       </c>
       <c r="B56">
-        <v>194</v>
-      </c>
-      <c r="C56" s="2">
-        <f t="shared" si="0"/>
-        <v>138.57142857142858</v>
-      </c>
-      <c r="D56" t="s">
-        <v>17</v>
+        <v>194.4</v>
+      </c>
+      <c r="C56" t="s">
+        <v>16</v>
+      </c>
+      <c r="D56">
+        <v>192783.5</v>
       </c>
       <c r="E56">
-        <v>192783.5</v>
+        <v>294664.96000000002</v>
       </c>
       <c r="F56">
-        <v>293730.77</v>
+        <v>98213.9</v>
       </c>
       <c r="G56">
-        <v>97235.69</v>
+        <v>196451.06</v>
       </c>
       <c r="H56">
-        <v>196495.08</v>
+        <v>1610.63</v>
       </c>
       <c r="I56">
-        <v>1549.25</v>
+        <v>99</v>
       </c>
       <c r="J56">
-        <v>99</v>
+        <v>67</v>
       </c>
       <c r="K56">
-        <v>67</v>
+        <v>62462.92</v>
       </c>
       <c r="L56">
-        <v>62194.82</v>
+        <v>57184.72</v>
       </c>
       <c r="M56">
-        <v>56933.98</v>
+        <v>24.82</v>
       </c>
       <c r="N56">
-        <v>24.71</v>
+        <v>201</v>
       </c>
       <c r="O56">
-        <v>197</v>
-      </c>
-      <c r="P56">
         <v>18</v>
       </c>
     </row>
-    <row r="57" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>1300</v>
       </c>
       <c r="B57">
-        <v>194</v>
-      </c>
-      <c r="C57" s="2">
-        <f t="shared" si="0"/>
-        <v>138.57142857142858</v>
-      </c>
-      <c r="D57" t="s">
+        <v>194.4</v>
+      </c>
+      <c r="C57" t="s">
+        <v>16</v>
+      </c>
+      <c r="D57">
+        <v>192783.5</v>
+      </c>
+      <c r="E57">
+        <v>294664.96000000002</v>
+      </c>
+      <c r="F57">
+        <v>97838.9</v>
+      </c>
+      <c r="G57">
+        <v>196826.06</v>
+      </c>
+      <c r="H57">
+        <v>1313.03</v>
+      </c>
+      <c r="I57">
+        <v>99</v>
+      </c>
+      <c r="J57">
+        <v>67</v>
+      </c>
+      <c r="K57">
+        <v>62837.919999999998</v>
+      </c>
+      <c r="L57">
+        <v>57482.32</v>
+      </c>
+      <c r="M57">
+        <v>23.03</v>
+      </c>
+      <c r="N57">
+        <v>190</v>
+      </c>
+      <c r="O57">
         <v>17</v>
       </c>
-      <c r="E57">
-        <v>192783.5</v>
-      </c>
-      <c r="F57">
-        <v>293730.77</v>
-      </c>
-      <c r="G57">
-        <v>96860.69</v>
-      </c>
-      <c r="H57">
-        <v>196870.08</v>
-      </c>
-      <c r="I57">
-        <v>1251.6500000000001</v>
-      </c>
-      <c r="J57">
-        <v>99</v>
-      </c>
-      <c r="K57">
-        <v>67</v>
-      </c>
-      <c r="L57">
-        <v>62569.82</v>
-      </c>
-      <c r="M57">
-        <v>57231.58</v>
-      </c>
-      <c r="N57">
-        <v>22.93</v>
-      </c>
-      <c r="O57">
-        <v>188</v>
-      </c>
-      <c r="P57">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="58" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="58" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>1400</v>
       </c>
       <c r="B58">
-        <v>194</v>
-      </c>
-      <c r="C58" s="2">
-        <f t="shared" si="0"/>
-        <v>138.57142857142858</v>
-      </c>
-      <c r="D58" t="s">
-        <v>17</v>
+        <v>194.4</v>
+      </c>
+      <c r="C58" t="s">
+        <v>16</v>
+      </c>
+      <c r="D58">
+        <v>192783.5</v>
       </c>
       <c r="E58">
-        <v>192783.5</v>
+        <v>294664.96000000002</v>
       </c>
       <c r="F58">
-        <v>293730.77</v>
+        <v>97463.9</v>
       </c>
       <c r="G58">
-        <v>96485.69</v>
+        <v>197201.06</v>
       </c>
       <c r="H58">
-        <v>197245.08</v>
+        <v>1015.43</v>
       </c>
       <c r="I58">
-        <v>954.05</v>
+        <v>99</v>
       </c>
       <c r="J58">
-        <v>100</v>
+        <v>67</v>
       </c>
       <c r="K58">
-        <v>67</v>
+        <v>63212.92</v>
       </c>
       <c r="L58">
-        <v>62944.82</v>
+        <v>57779.92</v>
       </c>
       <c r="M58">
-        <v>57529.18</v>
+        <v>21.5</v>
       </c>
       <c r="N58">
-        <v>21.4</v>
+        <v>156</v>
       </c>
       <c r="O58">
-        <v>154</v>
-      </c>
-      <c r="P58">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="59" spans="1:16" x14ac:dyDescent="0.2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="59" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>1500</v>
       </c>
       <c r="B59">
-        <v>194</v>
-      </c>
-      <c r="C59" s="2">
-        <f t="shared" si="0"/>
-        <v>138.57142857142858</v>
-      </c>
-      <c r="D59" t="s">
-        <v>17</v>
+        <v>194.4</v>
+      </c>
+      <c r="C59" t="s">
+        <v>16</v>
+      </c>
+      <c r="D59">
+        <v>192783.5</v>
       </c>
       <c r="E59">
-        <v>192783.5</v>
+        <v>294664.96000000002</v>
       </c>
       <c r="F59">
-        <v>293730.77</v>
+        <v>97088.9</v>
       </c>
       <c r="G59">
-        <v>96110.69</v>
+        <v>197576.06</v>
       </c>
       <c r="H59">
-        <v>197620.08</v>
+        <v>717.83</v>
       </c>
       <c r="I59">
-        <v>656.45</v>
+        <v>100</v>
       </c>
       <c r="J59">
-        <v>100</v>
+        <v>67</v>
       </c>
       <c r="K59">
-        <v>67</v>
+        <v>63587.92</v>
       </c>
       <c r="L59">
-        <v>63319.82</v>
+        <v>58077.52</v>
       </c>
       <c r="M59">
-        <v>57826.78</v>
+        <v>20.170000000000002</v>
       </c>
       <c r="N59">
-        <v>20.079999999999998</v>
+        <v>147</v>
       </c>
       <c r="O59">
-        <v>146</v>
-      </c>
-      <c r="P59">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="60" spans="1:16" x14ac:dyDescent="0.2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="60" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>1600</v>
       </c>
       <c r="B60">
-        <v>194</v>
-      </c>
-      <c r="C60" s="2">
-        <f t="shared" si="0"/>
-        <v>138.57142857142858</v>
-      </c>
-      <c r="D60" t="s">
-        <v>17</v>
+        <v>194.4</v>
+      </c>
+      <c r="C60" t="s">
+        <v>16</v>
+      </c>
+      <c r="D60">
+        <v>192783.5</v>
       </c>
       <c r="E60">
-        <v>192783.5</v>
+        <v>294664.96000000002</v>
       </c>
       <c r="F60">
-        <v>293730.77</v>
+        <v>96729.2</v>
       </c>
       <c r="G60">
-        <v>95763.25</v>
+        <v>197935.76</v>
       </c>
       <c r="H60">
-        <v>197967.52</v>
+        <v>434.33</v>
       </c>
       <c r="I60">
-        <v>384.25</v>
+        <v>100</v>
       </c>
       <c r="J60">
-        <v>100</v>
+        <v>67</v>
       </c>
       <c r="K60">
-        <v>67</v>
+        <v>63947.62</v>
       </c>
       <c r="L60">
-        <v>63667.25</v>
+        <v>58361.03</v>
       </c>
       <c r="M60">
-        <v>58098.98</v>
+        <v>19</v>
       </c>
       <c r="N60">
-        <v>18.91</v>
+        <v>115</v>
       </c>
       <c r="O60">
-        <v>96</v>
-      </c>
-      <c r="P60">
         <v>15</v>
       </c>
     </row>
-    <row r="61" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>1700</v>
       </c>
       <c r="B61">
-        <v>194</v>
-      </c>
-      <c r="C61" s="2">
-        <f t="shared" si="0"/>
-        <v>138.57142857142858</v>
-      </c>
-      <c r="D61" t="s">
-        <v>17</v>
+        <v>194.4</v>
+      </c>
+      <c r="C61" t="s">
+        <v>16</v>
+      </c>
+      <c r="D61">
+        <v>192783.5</v>
       </c>
       <c r="E61">
-        <v>192783.5</v>
+        <v>294664.96000000002</v>
       </c>
       <c r="F61">
-        <v>293730.77</v>
+        <v>96498.77</v>
       </c>
       <c r="G61">
-        <v>95564.14</v>
+        <v>198166.19</v>
       </c>
       <c r="H61">
-        <v>198166.63</v>
+        <v>269.97000000000003</v>
       </c>
       <c r="I61">
-        <v>248.75</v>
+        <v>100</v>
       </c>
       <c r="J61">
-        <v>100</v>
+        <v>67</v>
       </c>
       <c r="K61">
-        <v>67</v>
+        <v>64178.05</v>
       </c>
       <c r="L61">
-        <v>63866.36</v>
+        <v>58525.39</v>
       </c>
       <c r="M61">
-        <v>58234.48</v>
+        <v>17.93</v>
       </c>
       <c r="N61">
-        <v>17.84</v>
+        <v>85</v>
       </c>
       <c r="O61">
-        <v>85</v>
-      </c>
-      <c r="P61">
         <v>15</v>
       </c>
     </row>
-    <row r="62" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>1800</v>
       </c>
       <c r="B62">
-        <v>194</v>
-      </c>
-      <c r="C62" s="2">
-        <f t="shared" si="0"/>
-        <v>138.57142857142858</v>
-      </c>
-      <c r="D62" t="s">
-        <v>17</v>
+        <v>194.4</v>
+      </c>
+      <c r="C62" t="s">
+        <v>16</v>
+      </c>
+      <c r="D62">
+        <v>192783.5</v>
       </c>
       <c r="E62">
-        <v>192783.5</v>
+        <v>294664.96000000002</v>
       </c>
       <c r="F62">
-        <v>293730.77</v>
+        <v>96350.5</v>
       </c>
       <c r="G62">
-        <v>95423.49</v>
+        <v>198314.46</v>
       </c>
       <c r="H62">
-        <v>198307.29</v>
+        <v>181.33</v>
       </c>
       <c r="I62">
-        <v>167.12</v>
+        <v>100</v>
       </c>
       <c r="J62">
-        <v>100</v>
+        <v>67</v>
       </c>
       <c r="K62">
-        <v>68</v>
+        <v>64326.32</v>
       </c>
       <c r="L62">
-        <v>64007.02</v>
+        <v>58614.03</v>
       </c>
       <c r="M62">
-        <v>58316.11</v>
+        <v>16.96</v>
       </c>
       <c r="N62">
-        <v>16.87</v>
+        <v>57</v>
       </c>
       <c r="O62">
-        <v>57</v>
-      </c>
-      <c r="P62">
         <v>14</v>
       </c>
     </row>
-    <row r="63" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>1900</v>
       </c>
       <c r="B63">
-        <v>194</v>
-      </c>
-      <c r="C63" s="2">
-        <f t="shared" si="0"/>
-        <v>138.57142857142858</v>
-      </c>
-      <c r="D63" t="s">
-        <v>17</v>
+        <v>194.4</v>
+      </c>
+      <c r="C63" t="s">
+        <v>16</v>
+      </c>
+      <c r="D63">
+        <v>192783.5</v>
       </c>
       <c r="E63">
-        <v>192783.5</v>
+        <v>294664.96000000002</v>
       </c>
       <c r="F63">
-        <v>293730.77</v>
+        <v>96256.75</v>
       </c>
       <c r="G63">
-        <v>95329.74</v>
+        <v>198408.21</v>
       </c>
       <c r="H63">
-        <v>198401.04</v>
+        <v>142.93</v>
       </c>
       <c r="I63">
-        <v>128.72</v>
+        <v>100</v>
       </c>
       <c r="J63">
-        <v>100</v>
+        <v>67</v>
       </c>
       <c r="K63">
-        <v>68</v>
+        <v>64420.07</v>
       </c>
       <c r="L63">
-        <v>64100.77</v>
+        <v>58652.43</v>
       </c>
       <c r="M63">
-        <v>58354.51</v>
+        <v>16.079999999999998</v>
       </c>
       <c r="N63">
-        <v>16</v>
+        <v>56</v>
       </c>
       <c r="O63">
-        <v>56</v>
-      </c>
-      <c r="P63">
         <v>14</v>
       </c>
     </row>
-    <row r="64" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>2000</v>
       </c>
       <c r="B64">
-        <v>194</v>
-      </c>
-      <c r="C64" s="2">
-        <f t="shared" si="0"/>
-        <v>138.57142857142858</v>
-      </c>
-      <c r="D64" t="s">
-        <v>17</v>
+        <v>194.4</v>
+      </c>
+      <c r="C64" t="s">
+        <v>16</v>
+      </c>
+      <c r="D64">
+        <v>192783.5</v>
       </c>
       <c r="E64">
-        <v>192783.5</v>
+        <v>294664.96000000002</v>
       </c>
       <c r="F64">
-        <v>293730.77</v>
+        <v>96163</v>
       </c>
       <c r="G64">
-        <v>95235.99</v>
+        <v>198501.96</v>
       </c>
       <c r="H64">
-        <v>198494.79</v>
+        <v>104.53</v>
       </c>
       <c r="I64">
-        <v>90.32</v>
+        <v>100</v>
       </c>
       <c r="J64">
-        <v>100</v>
+        <v>67</v>
       </c>
       <c r="K64">
-        <v>68</v>
+        <v>64513.82</v>
       </c>
       <c r="L64">
-        <v>64194.52</v>
+        <v>58690.83</v>
       </c>
       <c r="M64">
-        <v>58392.91</v>
+        <v>15.28</v>
       </c>
       <c r="N64">
-        <v>15.21</v>
+        <v>49</v>
       </c>
       <c r="O64">
-        <v>42</v>
-      </c>
-      <c r="P64">
         <v>14</v>
       </c>
     </row>
-    <row r="65" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>2100</v>
       </c>
       <c r="B65">
-        <v>194</v>
-      </c>
-      <c r="C65" s="2">
-        <f t="shared" si="0"/>
-        <v>138.57142857142858</v>
-      </c>
-      <c r="D65" t="s">
-        <v>17</v>
+        <v>194.4</v>
+      </c>
+      <c r="C65" t="s">
+        <v>16</v>
+      </c>
+      <c r="D65">
+        <v>192783.5</v>
       </c>
       <c r="E65">
-        <v>192783.5</v>
+        <v>294664.96000000002</v>
       </c>
       <c r="F65">
-        <v>293730.77</v>
+        <v>96069.25</v>
       </c>
       <c r="G65">
-        <v>95142.24</v>
+        <v>198595.71</v>
       </c>
       <c r="H65">
-        <v>198588.54</v>
+        <v>66.13</v>
       </c>
       <c r="I65">
-        <v>51.92</v>
+        <v>100</v>
       </c>
       <c r="J65">
-        <v>100</v>
+        <v>67</v>
       </c>
       <c r="K65">
-        <v>68</v>
+        <v>64607.57</v>
       </c>
       <c r="L65">
-        <v>64288.27</v>
+        <v>58729.23</v>
       </c>
       <c r="M65">
-        <v>58431.31</v>
+        <v>14.57</v>
       </c>
       <c r="N65">
-        <v>14.49</v>
+        <v>28</v>
       </c>
       <c r="O65">
-        <v>28</v>
-      </c>
-      <c r="P65">
         <v>14</v>
       </c>
     </row>
-    <row r="66" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>2200</v>
       </c>
       <c r="B66">
-        <v>194</v>
-      </c>
-      <c r="C66" s="2">
-        <f t="shared" si="0"/>
-        <v>138.57142857142858</v>
-      </c>
-      <c r="D66" t="s">
-        <v>17</v>
+        <v>194.4</v>
+      </c>
+      <c r="C66" t="s">
+        <v>16</v>
+      </c>
+      <c r="D66">
+        <v>192783.5</v>
       </c>
       <c r="E66">
-        <v>192783.5</v>
+        <v>294664.96000000002</v>
       </c>
       <c r="F66">
-        <v>293730.77</v>
+        <v>95975.5</v>
       </c>
       <c r="G66">
-        <v>95048.49</v>
+        <v>198689.46</v>
       </c>
       <c r="H66">
-        <v>198682.29</v>
+        <v>27.73</v>
       </c>
       <c r="I66">
-        <v>13.52</v>
+        <v>100</v>
       </c>
       <c r="J66">
-        <v>100</v>
+        <v>67</v>
       </c>
       <c r="K66">
-        <v>68</v>
+        <v>64701.32</v>
       </c>
       <c r="L66">
-        <v>64382.02</v>
+        <v>58767.63</v>
       </c>
       <c r="M66">
-        <v>58469.71</v>
+        <v>13.91</v>
       </c>
       <c r="N66">
-        <v>13.84</v>
+        <v>20</v>
       </c>
       <c r="O66">
         <v>10</v>
       </c>
-      <c r="P66">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="67" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="67" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>2300</v>
       </c>
       <c r="B67">
-        <v>194</v>
-      </c>
-      <c r="C67" s="2">
-        <f t="shared" ref="C67" si="1">B67/1.4</f>
-        <v>138.57142857142858</v>
-      </c>
-      <c r="D67" t="s">
-        <v>17</v>
+        <v>194.4</v>
+      </c>
+      <c r="C67" t="s">
+        <v>16</v>
+      </c>
+      <c r="D67">
+        <v>192783.5</v>
       </c>
       <c r="E67">
-        <v>192783.5</v>
+        <v>294664.96000000002</v>
       </c>
       <c r="F67">
-        <v>293730.77</v>
+        <v>95893.34</v>
       </c>
       <c r="G67">
-        <v>94981.73</v>
+        <v>198771.62</v>
       </c>
       <c r="H67">
-        <v>198749.04</v>
+        <v>0</v>
       </c>
       <c r="I67">
+        <v>100</v>
+      </c>
+      <c r="J67">
+        <v>67</v>
+      </c>
+      <c r="K67">
+        <v>64783.48</v>
+      </c>
+      <c r="L67">
+        <v>58795.360000000001</v>
+      </c>
+      <c r="M67">
+        <v>13.31</v>
+      </c>
+      <c r="N67">
         <v>0</v>
       </c>
-      <c r="J67">
-        <v>100</v>
-      </c>
-      <c r="K67">
-        <v>68</v>
-      </c>
-      <c r="L67">
-        <v>64448.78</v>
-      </c>
-      <c r="M67">
-        <v>58483.23</v>
-      </c>
-      <c r="N67">
-        <v>13.24</v>
-      </c>
       <c r="O67">
-        <v>0</v>
-      </c>
-      <c r="P67">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
second run - 2 canopies
</commit_message>
<xml_diff>
--- a/(client deliverable)SGWS_Scenario_comparison.xlsx
+++ b/(client deliverable)SGWS_Scenario_comparison.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mykolaturchak/PycharmProjects/Valuestack/sgws_microgrid/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE18ACD4-C135-9C4C-8046-FD538DBC4AAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84791D71-E319-4146-85C6-3E70DADCB5D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="160" yWindow="660" windowWidth="28480" windowHeight="16120" xr2:uid="{BBC9B5F1-E85E-E64A-A67A-0CEF0D7F3E37}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="19">
   <si>
     <t>total_load_kwh</t>
   </si>
@@ -87,6 +87,9 @@
   </si>
   <si>
     <t>Low</t>
+  </si>
+  <si>
+    <t>power_kw</t>
   </si>
 </sst>
 </file>
@@ -948,3165 +951,3168 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CC78E7F-F823-9A45-863E-EBED49755FF5}">
-  <dimension ref="A1:O67"/>
+  <dimension ref="A1:P67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="I52" sqref="I52"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="16" max="16" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="13.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>12</v>
       </c>
       <c r="B1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" t="s">
         <v>13</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>14</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>0</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>1</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>2</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>3</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>4</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>5</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>6</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>7</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>8</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>9</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>10</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>100</v>
       </c>
-      <c r="B2">
+      <c r="C2">
         <v>259.2</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>15</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <v>135543.5</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>392886.42</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>264576.46999999997</v>
       </c>
-      <c r="G2">
+      <c r="H2">
         <v>128309.95</v>
       </c>
-      <c r="H2">
+      <c r="I2">
         <v>9229.33</v>
       </c>
-      <c r="I2">
+      <c r="J2">
         <v>93</v>
       </c>
-      <c r="J2">
+      <c r="K2">
         <v>33</v>
       </c>
-      <c r="K2">
+      <c r="L2">
         <v>25946.2</v>
       </c>
-      <c r="L2">
+      <c r="M2">
         <v>23950.41</v>
       </c>
-      <c r="M2">
+      <c r="N2">
         <v>124.54</v>
       </c>
-      <c r="N2">
+      <c r="O2">
         <v>3261</v>
       </c>
-      <c r="O2">
+      <c r="P2">
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>200</v>
       </c>
-      <c r="B3">
+      <c r="C3">
         <v>259.2</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>15</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <v>135543.5</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>392886.42</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>257055.69</v>
       </c>
-      <c r="G3">
+      <c r="H3">
         <v>135830.73000000001</v>
       </c>
-      <c r="H3">
+      <c r="I3">
         <v>2324.31</v>
       </c>
-      <c r="I3">
+      <c r="J3">
         <v>98</v>
       </c>
-      <c r="J3">
+      <c r="K3">
         <v>35</v>
       </c>
-      <c r="K3">
+      <c r="L3">
         <v>33466.980000000003</v>
       </c>
-      <c r="L3">
+      <c r="M3">
         <v>30855.439999999999</v>
       </c>
-      <c r="M3">
+      <c r="N3">
         <v>80.319999999999993</v>
       </c>
-      <c r="N3">
+      <c r="O3">
         <v>653</v>
       </c>
-      <c r="O3">
+      <c r="P3">
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>300</v>
       </c>
-      <c r="B4">
+      <c r="C4">
         <v>259.2</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>15</v>
       </c>
-      <c r="D4">
+      <c r="E4">
         <v>135543.5</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <v>392886.42</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>255348.54</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>137537.88</v>
       </c>
-      <c r="H4">
+      <c r="I4">
         <v>799</v>
       </c>
-      <c r="I4">
+      <c r="J4">
         <v>99</v>
       </c>
-      <c r="J4">
+      <c r="K4">
         <v>35</v>
       </c>
-      <c r="K4">
+      <c r="L4">
         <v>35174.129999999997</v>
       </c>
-      <c r="L4">
+      <c r="M4">
         <v>32380.75</v>
       </c>
-      <c r="M4">
+      <c r="N4">
         <v>56.22</v>
       </c>
-      <c r="N4">
+      <c r="O4">
         <v>215</v>
       </c>
-      <c r="O4">
+      <c r="P4">
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>400</v>
       </c>
-      <c r="B5">
+      <c r="C5">
         <v>259.2</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>15</v>
       </c>
-      <c r="D5">
+      <c r="E5">
         <v>135543.5</v>
       </c>
-      <c r="E5">
+      <c r="F5">
         <v>392886.42</v>
       </c>
-      <c r="F5">
+      <c r="G5">
         <v>254807.99</v>
       </c>
-      <c r="G5">
+      <c r="H5">
         <v>138078.43</v>
       </c>
-      <c r="H5">
+      <c r="I5">
         <v>348.83</v>
       </c>
-      <c r="I5">
+      <c r="J5">
         <v>100</v>
       </c>
-      <c r="J5">
+      <c r="K5">
         <v>35</v>
       </c>
-      <c r="K5">
+      <c r="L5">
         <v>35714.68</v>
       </c>
-      <c r="L5">
+      <c r="M5">
         <v>32830.92</v>
       </c>
-      <c r="M5">
+      <c r="N5">
         <v>42.75</v>
       </c>
-      <c r="N5">
+      <c r="O5">
         <v>77</v>
       </c>
-      <c r="O5">
+      <c r="P5">
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>500</v>
       </c>
-      <c r="B6">
+      <c r="C6">
         <v>259.2</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>15</v>
       </c>
-      <c r="D6">
+      <c r="E6">
         <v>135543.5</v>
       </c>
-      <c r="E6">
+      <c r="F6">
         <v>392886.42</v>
       </c>
-      <c r="F6">
+      <c r="G6">
         <v>254594.37</v>
       </c>
-      <c r="G6">
+      <c r="H6">
         <v>138292.04999999999</v>
       </c>
-      <c r="H6">
+      <c r="I6">
         <v>199.96</v>
       </c>
-      <c r="I6">
+      <c r="J6">
         <v>100</v>
       </c>
-      <c r="J6">
+      <c r="K6">
         <v>35</v>
       </c>
-      <c r="K6">
+      <c r="L6">
         <v>35928.29</v>
       </c>
-      <c r="L6">
+      <c r="M6">
         <v>32979.79</v>
       </c>
-      <c r="M6">
+      <c r="N6">
         <v>34.35</v>
       </c>
-      <c r="N6">
+      <c r="O6">
         <v>32</v>
       </c>
-      <c r="O6">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P6">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>600</v>
       </c>
-      <c r="B7">
+      <c r="C7">
         <v>259.2</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>15</v>
       </c>
-      <c r="D7">
+      <c r="E7">
         <v>135543.5</v>
       </c>
-      <c r="E7">
+      <c r="F7">
         <v>392886.42</v>
       </c>
-      <c r="F7">
+      <c r="G7">
         <v>254448.54</v>
       </c>
-      <c r="G7">
+      <c r="H7">
         <v>138437.88</v>
       </c>
-      <c r="H7">
+      <c r="I7">
         <v>113.56</v>
       </c>
-      <c r="I7">
+      <c r="J7">
         <v>100</v>
       </c>
-      <c r="J7">
+      <c r="K7">
         <v>35</v>
       </c>
-      <c r="K7">
+      <c r="L7">
         <v>36074.129999999997</v>
       </c>
-      <c r="L7">
+      <c r="M7">
         <v>33066.19</v>
       </c>
-      <c r="M7">
+      <c r="N7">
         <v>28.7</v>
       </c>
-      <c r="N7">
+      <c r="O7">
         <v>29</v>
       </c>
-      <c r="O7">
+      <c r="P7">
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>700</v>
       </c>
-      <c r="B8">
+      <c r="C8">
         <v>259.2</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>15</v>
       </c>
-      <c r="D8">
+      <c r="E8">
         <v>135543.5</v>
       </c>
-      <c r="E8">
+      <c r="F8">
         <v>392886.42</v>
       </c>
-      <c r="F8">
+      <c r="G8">
         <v>254302.71</v>
       </c>
-      <c r="G8">
+      <c r="H8">
         <v>138583.71</v>
       </c>
-      <c r="H8">
+      <c r="I8">
         <v>27.16</v>
       </c>
-      <c r="I8">
+      <c r="J8">
         <v>100</v>
       </c>
-      <c r="J8">
+      <c r="K8">
         <v>35</v>
       </c>
-      <c r="K8">
+      <c r="L8">
         <v>36219.96</v>
       </c>
-      <c r="L8">
+      <c r="M8">
         <v>33152.589999999997</v>
       </c>
-      <c r="M8">
+      <c r="N8">
         <v>24.67</v>
       </c>
-      <c r="N8">
+      <c r="O8">
         <v>19</v>
       </c>
-      <c r="O8">
+      <c r="P8">
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>800</v>
       </c>
-      <c r="B9">
+      <c r="C9">
         <v>259.2</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>15</v>
       </c>
-      <c r="D9">
+      <c r="E9">
         <v>135543.5</v>
       </c>
-      <c r="E9">
+      <c r="F9">
         <v>392886.42</v>
       </c>
-      <c r="F9">
+      <c r="G9">
         <v>254221.15</v>
       </c>
-      <c r="G9">
+      <c r="H9">
         <v>138665.26999999999</v>
       </c>
-      <c r="H9">
+      <c r="I9">
         <v>0</v>
       </c>
-      <c r="I9">
+      <c r="J9">
         <v>100</v>
       </c>
-      <c r="J9">
+      <c r="K9">
         <v>35</v>
       </c>
-      <c r="K9">
+      <c r="L9">
         <v>36301.519999999997</v>
       </c>
-      <c r="L9">
+      <c r="M9">
         <v>33179.75</v>
       </c>
-      <c r="M9">
+      <c r="N9">
         <v>21.6</v>
-      </c>
-      <c r="N9">
-        <v>0</v>
       </c>
       <c r="O9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>100</v>
       </c>
-      <c r="B10">
+      <c r="C10">
         <v>259.2</v>
       </c>
-      <c r="C10" t="s">
-        <v>16</v>
-      </c>
-      <c r="D10">
+      <c r="D10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10">
         <v>192783.5</v>
       </c>
-      <c r="E10">
+      <c r="F10">
         <v>392886.42</v>
       </c>
-      <c r="F10">
+      <c r="G10">
         <v>219553.29</v>
       </c>
-      <c r="G10">
+      <c r="H10">
         <v>173333.13</v>
       </c>
-      <c r="H10">
+      <c r="I10">
         <v>21647.53</v>
       </c>
-      <c r="I10">
+      <c r="J10">
         <v>89</v>
       </c>
-      <c r="J10">
+      <c r="K10">
         <v>44</v>
       </c>
-      <c r="K10">
+      <c r="L10">
         <v>28514.78</v>
       </c>
-      <c r="L10">
+      <c r="M10">
         <v>26317.62</v>
       </c>
-      <c r="M10">
+      <c r="N10">
         <v>136.87</v>
       </c>
-      <c r="N10">
+      <c r="O10">
         <v>4815</v>
       </c>
-      <c r="O10">
+      <c r="P10">
         <v>36</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>200</v>
       </c>
-      <c r="B11">
+      <c r="C11">
         <v>259.2</v>
       </c>
-      <c r="C11" t="s">
-        <v>16</v>
-      </c>
-      <c r="D11">
+      <c r="D11" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11">
         <v>192783.5</v>
       </c>
-      <c r="E11">
+      <c r="F11">
         <v>392886.42</v>
       </c>
-      <c r="F11">
+      <c r="G11">
         <v>206923.61</v>
       </c>
-      <c r="G11">
+      <c r="H11">
         <v>185962.81</v>
       </c>
-      <c r="H11">
+      <c r="I11">
         <v>9998.23</v>
       </c>
-      <c r="I11">
+      <c r="J11">
         <v>95</v>
       </c>
-      <c r="J11">
+      <c r="K11">
         <v>47</v>
       </c>
-      <c r="K11">
+      <c r="L11">
         <v>41144.46</v>
       </c>
-      <c r="L11">
+      <c r="M11">
         <v>37966.93</v>
       </c>
-      <c r="M11">
+      <c r="N11">
         <v>98.75</v>
       </c>
-      <c r="N11">
+      <c r="O11">
         <v>2198</v>
       </c>
-      <c r="O11">
+      <c r="P11">
         <v>36</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>300</v>
       </c>
-      <c r="B12">
+      <c r="C12">
         <v>259.2</v>
       </c>
-      <c r="C12" t="s">
-        <v>16</v>
-      </c>
-      <c r="D12">
+      <c r="D12" t="s">
+        <v>16</v>
+      </c>
+      <c r="E12">
         <v>192783.5</v>
       </c>
-      <c r="E12">
+      <c r="F12">
         <v>392886.42</v>
       </c>
-      <c r="F12">
+      <c r="G12">
         <v>202351.82</v>
       </c>
-      <c r="G12">
+      <c r="H12">
         <v>190534.6</v>
       </c>
-      <c r="H12">
+      <c r="I12">
         <v>5832.86</v>
       </c>
-      <c r="I12">
+      <c r="J12">
         <v>97</v>
       </c>
-      <c r="J12">
+      <c r="K12">
         <v>48</v>
       </c>
-      <c r="K12">
+      <c r="L12">
         <v>45716.25</v>
       </c>
-      <c r="L12">
+      <c r="M12">
         <v>42132.29</v>
       </c>
-      <c r="M12">
+      <c r="N12">
         <v>73.150000000000006</v>
       </c>
-      <c r="N12">
+      <c r="O12">
         <v>1116</v>
       </c>
-      <c r="O12">
+      <c r="P12">
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>400</v>
       </c>
-      <c r="B13">
+      <c r="C13">
         <v>259.2</v>
       </c>
-      <c r="C13" t="s">
-        <v>16</v>
-      </c>
-      <c r="D13">
+      <c r="D13" t="s">
+        <v>16</v>
+      </c>
+      <c r="E13">
         <v>192783.5</v>
       </c>
-      <c r="E13">
+      <c r="F13">
         <v>392886.42</v>
       </c>
-      <c r="F13">
+      <c r="G13">
         <v>200267.44</v>
       </c>
-      <c r="G13">
+      <c r="H13">
         <v>192618.98</v>
       </c>
-      <c r="H13">
+      <c r="I13">
         <v>3959.9</v>
       </c>
-      <c r="I13">
+      <c r="J13">
         <v>98</v>
       </c>
-      <c r="J13">
+      <c r="K13">
         <v>49</v>
       </c>
-      <c r="K13">
+      <c r="L13">
         <v>47800.63</v>
       </c>
-      <c r="L13">
+      <c r="M13">
         <v>44005.25</v>
       </c>
-      <c r="M13">
+      <c r="N13">
         <v>57.3</v>
       </c>
-      <c r="N13">
+      <c r="O13">
         <v>692</v>
       </c>
-      <c r="O13">
+      <c r="P13">
         <v>36</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>500</v>
       </c>
-      <c r="B14">
+      <c r="C14">
         <v>259.2</v>
       </c>
-      <c r="C14" t="s">
-        <v>16</v>
-      </c>
-      <c r="D14">
+      <c r="D14" t="s">
+        <v>16</v>
+      </c>
+      <c r="E14">
         <v>192783.5</v>
       </c>
-      <c r="E14">
+      <c r="F14">
         <v>392886.42</v>
       </c>
-      <c r="F14">
+      <c r="G14">
         <v>198702.8</v>
       </c>
-      <c r="G14">
+      <c r="H14">
         <v>194183.62</v>
       </c>
-      <c r="H14">
+      <c r="I14">
         <v>2565.9299999999998</v>
       </c>
-      <c r="I14">
+      <c r="J14">
         <v>99</v>
       </c>
-      <c r="J14">
+      <c r="K14">
         <v>49</v>
       </c>
-      <c r="K14">
+      <c r="L14">
         <v>49365.27</v>
       </c>
-      <c r="L14">
+      <c r="M14">
         <v>45399.22</v>
       </c>
-      <c r="M14">
+      <c r="N14">
         <v>47.29</v>
       </c>
-      <c r="N14">
+      <c r="O14">
         <v>508</v>
       </c>
-      <c r="O14">
+      <c r="P14">
         <v>36</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>600</v>
       </c>
-      <c r="B15">
+      <c r="C15">
         <v>259.2</v>
       </c>
-      <c r="C15" t="s">
-        <v>16</v>
-      </c>
-      <c r="D15">
+      <c r="D15" t="s">
+        <v>16</v>
+      </c>
+      <c r="E15">
         <v>192783.5</v>
       </c>
-      <c r="E15">
+      <c r="F15">
         <v>392886.42</v>
       </c>
-      <c r="F15">
+      <c r="G15">
         <v>197597.57</v>
       </c>
-      <c r="G15">
+      <c r="H15">
         <v>195288.85</v>
       </c>
-      <c r="H15">
+      <c r="I15">
         <v>1595.35</v>
       </c>
-      <c r="I15">
+      <c r="J15">
         <v>99</v>
       </c>
-      <c r="J15">
+      <c r="K15">
         <v>50</v>
       </c>
-      <c r="K15">
+      <c r="L15">
         <v>50470.5</v>
       </c>
-      <c r="L15">
+      <c r="M15">
         <v>46369.81</v>
       </c>
-      <c r="M15">
+      <c r="N15">
         <v>40.25</v>
       </c>
-      <c r="N15">
+      <c r="O15">
         <v>292</v>
       </c>
-      <c r="O15">
+      <c r="P15">
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>700</v>
       </c>
-      <c r="B16">
+      <c r="C16">
         <v>259.2</v>
       </c>
-      <c r="C16" t="s">
-        <v>16</v>
-      </c>
-      <c r="D16">
+      <c r="D16" t="s">
+        <v>16</v>
+      </c>
+      <c r="E16">
         <v>192783.5</v>
       </c>
-      <c r="E16">
+      <c r="F16">
         <v>392886.42</v>
       </c>
-      <c r="F16">
+      <c r="G16">
         <v>196872.43</v>
       </c>
-      <c r="G16">
+      <c r="H16">
         <v>196013.99</v>
       </c>
-      <c r="H16">
+      <c r="I16">
         <v>975.06</v>
       </c>
-      <c r="I16">
+      <c r="J16">
         <v>99</v>
       </c>
-      <c r="J16">
+      <c r="K16">
         <v>50</v>
       </c>
-      <c r="K16">
+      <c r="L16">
         <v>51195.64</v>
       </c>
-      <c r="L16">
+      <c r="M16">
         <v>46990.1</v>
       </c>
-      <c r="M16">
+      <c r="N16">
         <v>34.96</v>
       </c>
-      <c r="N16">
+      <c r="O16">
         <v>105</v>
       </c>
-      <c r="O16">
+      <c r="P16">
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>800</v>
       </c>
-      <c r="B17">
+      <c r="C17">
         <v>259.2</v>
       </c>
-      <c r="C17" t="s">
-        <v>16</v>
-      </c>
-      <c r="D17">
+      <c r="D17" t="s">
+        <v>16</v>
+      </c>
+      <c r="E17">
         <v>192783.5</v>
       </c>
-      <c r="E17">
+      <c r="F17">
         <v>392886.42</v>
       </c>
-      <c r="F17">
+      <c r="G17">
         <v>196587.41</v>
       </c>
-      <c r="G17">
+      <c r="H17">
         <v>196299.01</v>
       </c>
-      <c r="H17">
+      <c r="I17">
         <v>760.38</v>
       </c>
-      <c r="I17">
+      <c r="J17">
         <v>100</v>
       </c>
-      <c r="J17">
+      <c r="K17">
         <v>50</v>
       </c>
-      <c r="K17">
+      <c r="L17">
         <v>51480.67</v>
       </c>
-      <c r="L17">
+      <c r="M17">
         <v>47204.77</v>
       </c>
-      <c r="M17">
+      <c r="N17">
         <v>30.73</v>
       </c>
-      <c r="N17">
+      <c r="O17">
         <v>69</v>
       </c>
-      <c r="O17">
+      <c r="P17">
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>900</v>
       </c>
-      <c r="B18">
+      <c r="C18">
         <v>259.2</v>
       </c>
-      <c r="C18" t="s">
-        <v>16</v>
-      </c>
-      <c r="D18">
+      <c r="D18" t="s">
+        <v>16</v>
+      </c>
+      <c r="E18">
         <v>192783.5</v>
       </c>
-      <c r="E18">
+      <c r="F18">
         <v>392886.42</v>
       </c>
-      <c r="F18">
+      <c r="G18">
         <v>196347.82</v>
       </c>
-      <c r="G18">
+      <c r="H18">
         <v>196538.6</v>
       </c>
-      <c r="H18">
+      <c r="I18">
         <v>587.58000000000004</v>
       </c>
-      <c r="I18">
+      <c r="J18">
         <v>100</v>
       </c>
-      <c r="J18">
+      <c r="K18">
         <v>50</v>
       </c>
-      <c r="K18">
+      <c r="L18">
         <v>51720.25</v>
       </c>
-      <c r="L18">
+      <c r="M18">
         <v>47377.57</v>
       </c>
-      <c r="M18">
+      <c r="N18">
         <v>27.42</v>
       </c>
-      <c r="N18">
+      <c r="O18">
         <v>63</v>
       </c>
-      <c r="O18">
+      <c r="P18">
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>1000</v>
       </c>
-      <c r="B19">
+      <c r="C19">
         <v>259.2</v>
       </c>
-      <c r="C19" t="s">
-        <v>16</v>
-      </c>
-      <c r="D19">
+      <c r="D19" t="s">
+        <v>16</v>
+      </c>
+      <c r="E19">
         <v>192783.5</v>
       </c>
-      <c r="E19">
+      <c r="F19">
         <v>392886.42</v>
       </c>
-      <c r="F19">
+      <c r="G19">
         <v>196108.24</v>
       </c>
-      <c r="G19">
+      <c r="H19">
         <v>196778.18</v>
       </c>
-      <c r="H19">
+      <c r="I19">
         <v>414.78</v>
       </c>
-      <c r="I19">
+      <c r="J19">
         <v>100</v>
       </c>
-      <c r="J19">
+      <c r="K19">
         <v>50</v>
       </c>
-      <c r="K19">
+      <c r="L19">
         <v>51959.83</v>
       </c>
-      <c r="L19">
+      <c r="M19">
         <v>47550.37</v>
       </c>
-      <c r="M19">
+      <c r="N19">
         <v>24.77</v>
       </c>
-      <c r="N19">
+      <c r="O19">
         <v>59</v>
       </c>
-      <c r="O19">
+      <c r="P19">
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>1100</v>
       </c>
-      <c r="B20">
+      <c r="C20">
         <v>259.2</v>
       </c>
-      <c r="C20" t="s">
-        <v>16</v>
-      </c>
-      <c r="D20">
+      <c r="D20" t="s">
+        <v>16</v>
+      </c>
+      <c r="E20">
         <v>192783.5</v>
       </c>
-      <c r="E20">
+      <c r="F20">
         <v>392886.42</v>
       </c>
-      <c r="F20">
+      <c r="G20">
         <v>195909.92</v>
       </c>
-      <c r="G20">
+      <c r="H20">
         <v>196976.5</v>
       </c>
-      <c r="H20">
+      <c r="I20">
         <v>280.01</v>
       </c>
-      <c r="I20">
+      <c r="J20">
         <v>100</v>
       </c>
-      <c r="J20">
+      <c r="K20">
         <v>50</v>
       </c>
-      <c r="K20">
+      <c r="L20">
         <v>52158.15</v>
       </c>
-      <c r="L20">
+      <c r="M20">
         <v>47685.14</v>
       </c>
-      <c r="M20">
+      <c r="N20">
         <v>22.58</v>
       </c>
-      <c r="N20">
+      <c r="O20">
         <v>32</v>
       </c>
-      <c r="O20">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P20">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>1200</v>
       </c>
-      <c r="B21">
+      <c r="C21">
         <v>259.2</v>
       </c>
-      <c r="C21" t="s">
-        <v>16</v>
-      </c>
-      <c r="D21">
+      <c r="D21" t="s">
+        <v>16</v>
+      </c>
+      <c r="E21">
         <v>192783.5</v>
       </c>
-      <c r="E21">
+      <c r="F21">
         <v>392886.42</v>
       </c>
-      <c r="F21">
+      <c r="G21">
         <v>195764.08</v>
       </c>
-      <c r="G21">
+      <c r="H21">
         <v>197122.34</v>
       </c>
-      <c r="H21">
+      <c r="I21">
         <v>193.61</v>
       </c>
-      <c r="I21">
+      <c r="J21">
         <v>100</v>
       </c>
-      <c r="J21">
+      <c r="K21">
         <v>50</v>
       </c>
-      <c r="K21">
+      <c r="L21">
         <v>52303.99</v>
       </c>
-      <c r="L21">
+      <c r="M21">
         <v>47771.54</v>
       </c>
-      <c r="M21">
+      <c r="N21">
         <v>20.73</v>
       </c>
-      <c r="N21">
+      <c r="O21">
         <v>30</v>
       </c>
-      <c r="O21">
+      <c r="P21">
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>1300</v>
       </c>
-      <c r="B22">
+      <c r="C22">
         <v>259.2</v>
       </c>
-      <c r="C22" t="s">
-        <v>16</v>
-      </c>
-      <c r="D22">
+      <c r="D22" t="s">
+        <v>16</v>
+      </c>
+      <c r="E22">
         <v>192783.5</v>
       </c>
-      <c r="E22">
+      <c r="F22">
         <v>392886.42</v>
       </c>
-      <c r="F22">
+      <c r="G22">
         <v>195618.25</v>
       </c>
-      <c r="G22">
+      <c r="H22">
         <v>197268.17</v>
       </c>
-      <c r="H22">
+      <c r="I22">
         <v>107.21</v>
       </c>
-      <c r="I22">
+      <c r="J22">
         <v>100</v>
       </c>
-      <c r="J22">
+      <c r="K22">
         <v>50</v>
       </c>
-      <c r="K22">
+      <c r="L22">
         <v>52449.82</v>
       </c>
-      <c r="L22">
+      <c r="M22">
         <v>47857.94</v>
       </c>
-      <c r="M22">
+      <c r="N22">
         <v>19.170000000000002</v>
       </c>
-      <c r="N22">
+      <c r="O22">
         <v>28</v>
       </c>
-      <c r="O22">
+      <c r="P22">
         <v>14</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>1400</v>
       </c>
-      <c r="B23">
+      <c r="C23">
         <v>259.2</v>
       </c>
-      <c r="C23" t="s">
-        <v>16</v>
-      </c>
-      <c r="D23">
+      <c r="D23" t="s">
+        <v>16</v>
+      </c>
+      <c r="E23">
         <v>192783.5</v>
       </c>
-      <c r="E23">
+      <c r="F23">
         <v>392886.42</v>
       </c>
-      <c r="F23">
+      <c r="G23">
         <v>195472.42</v>
       </c>
-      <c r="G23">
+      <c r="H23">
         <v>197414</v>
       </c>
-      <c r="H23">
+      <c r="I23">
         <v>20.81</v>
       </c>
-      <c r="I23">
+      <c r="J23">
         <v>100</v>
       </c>
-      <c r="J23">
+      <c r="K23">
         <v>50</v>
       </c>
-      <c r="K23">
+      <c r="L23">
         <v>52595.65</v>
       </c>
-      <c r="L23">
+      <c r="M23">
         <v>47944.34</v>
       </c>
-      <c r="M23">
+      <c r="N23">
         <v>17.84</v>
       </c>
-      <c r="N23">
+      <c r="O23">
         <v>14</v>
       </c>
-      <c r="O23">
+      <c r="P23">
         <v>7</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>1500</v>
       </c>
-      <c r="B24">
+      <c r="C24">
         <v>259.2</v>
       </c>
-      <c r="C24" t="s">
-        <v>16</v>
-      </c>
-      <c r="D24">
+      <c r="D24" t="s">
+        <v>16</v>
+      </c>
+      <c r="E24">
         <v>192783.5</v>
       </c>
-      <c r="E24">
+      <c r="F24">
         <v>392886.42</v>
       </c>
-      <c r="F24">
+      <c r="G24">
         <v>195397.76000000001</v>
       </c>
-      <c r="G24">
+      <c r="H24">
         <v>197488.66</v>
       </c>
-      <c r="H24">
+      <c r="I24">
         <v>0</v>
       </c>
-      <c r="I24">
+      <c r="J24">
         <v>100</v>
       </c>
-      <c r="J24">
+      <c r="K24">
         <v>50</v>
       </c>
-      <c r="K24">
+      <c r="L24">
         <v>52670.32</v>
       </c>
-      <c r="L24">
+      <c r="M24">
         <v>47965.15</v>
       </c>
-      <c r="M24">
+      <c r="N24">
         <v>16.649999999999999</v>
-      </c>
-      <c r="N24">
-        <v>0</v>
       </c>
       <c r="O24">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>100</v>
       </c>
-      <c r="B25">
+      <c r="C25">
         <v>259.2</v>
       </c>
-      <c r="C25" t="s">
+      <c r="D25" t="s">
         <v>17</v>
       </c>
-      <c r="D25">
+      <c r="E25">
         <v>98582.5</v>
       </c>
-      <c r="E25">
+      <c r="F25">
         <v>392886.42</v>
       </c>
-      <c r="F25">
+      <c r="G25">
         <v>294489.53000000003</v>
       </c>
-      <c r="G25">
+      <c r="H25">
         <v>98396.89</v>
       </c>
-      <c r="H25">
+      <c r="I25">
         <v>1883.54</v>
       </c>
-      <c r="I25">
+      <c r="J25">
         <v>98</v>
       </c>
-      <c r="J25">
+      <c r="K25">
         <v>25</v>
       </c>
-      <c r="K25">
+      <c r="L25">
         <v>21750.87</v>
       </c>
-      <c r="L25">
+      <c r="M25">
         <v>20052.939999999999</v>
       </c>
-      <c r="M25">
+      <c r="N25">
         <v>104.4</v>
       </c>
-      <c r="N25">
+      <c r="O25">
         <v>844</v>
       </c>
-      <c r="O25">
+      <c r="P25">
         <v>20</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>200</v>
       </c>
-      <c r="B26">
+      <c r="C26">
         <v>259.2</v>
       </c>
-      <c r="C26" t="s">
+      <c r="D26" t="s">
         <v>17</v>
       </c>
-      <c r="D26">
+      <c r="E26">
         <v>98582.5</v>
       </c>
-      <c r="E26">
+      <c r="F26">
         <v>392886.42</v>
       </c>
-      <c r="F26">
+      <c r="G26">
         <v>292754.5</v>
       </c>
-      <c r="G26">
+      <c r="H26">
         <v>100131.91</v>
       </c>
-      <c r="H26">
+      <c r="I26">
         <v>332.54</v>
       </c>
-      <c r="I26">
+      <c r="J26">
         <v>100</v>
       </c>
-      <c r="J26">
+      <c r="K26">
         <v>25</v>
       </c>
-      <c r="K26">
+      <c r="L26">
         <v>23485.9</v>
       </c>
-      <c r="L26">
+      <c r="M26">
         <v>21603.94</v>
       </c>
-      <c r="M26">
+      <c r="N26">
         <v>56.26</v>
       </c>
-      <c r="N26">
+      <c r="O26">
         <v>108</v>
       </c>
-      <c r="O26">
+      <c r="P26">
         <v>18</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>300</v>
       </c>
-      <c r="B27">
+      <c r="C27">
         <v>259.2</v>
       </c>
-      <c r="C27" t="s">
+      <c r="D27" t="s">
         <v>17</v>
       </c>
-      <c r="D27">
+      <c r="E27">
         <v>98582.5</v>
       </c>
-      <c r="E27">
+      <c r="F27">
         <v>392886.42</v>
       </c>
-      <c r="F27">
+      <c r="G27">
         <v>292489.09999999998</v>
       </c>
-      <c r="G27">
+      <c r="H27">
         <v>100397.32</v>
       </c>
-      <c r="H27">
+      <c r="I27">
         <v>135.94999999999999</v>
       </c>
-      <c r="I27">
+      <c r="J27">
         <v>100</v>
       </c>
-      <c r="J27">
+      <c r="K27">
         <v>26</v>
       </c>
-      <c r="K27">
+      <c r="L27">
         <v>23751.3</v>
       </c>
-      <c r="L27">
+      <c r="M27">
         <v>21800.53</v>
       </c>
-      <c r="M27">
+      <c r="N27">
         <v>37.85</v>
       </c>
-      <c r="N27">
+      <c r="O27">
         <v>31</v>
       </c>
-      <c r="O27">
+      <c r="P27">
         <v>15</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>400</v>
       </c>
-      <c r="B28">
+      <c r="C28">
         <v>259.2</v>
       </c>
-      <c r="C28" t="s">
+      <c r="D28" t="s">
         <v>17</v>
       </c>
-      <c r="D28">
+      <c r="E28">
         <v>98582.5</v>
       </c>
-      <c r="E28">
+      <c r="F28">
         <v>392886.42</v>
       </c>
-      <c r="F28">
+      <c r="G28">
         <v>292343.27</v>
       </c>
-      <c r="G28">
+      <c r="H28">
         <v>100543.15</v>
       </c>
-      <c r="H28">
+      <c r="I28">
         <v>49.55</v>
       </c>
-      <c r="I28">
+      <c r="J28">
         <v>100</v>
       </c>
-      <c r="J28">
+      <c r="K28">
         <v>26</v>
       </c>
-      <c r="K28">
+      <c r="L28">
         <v>23897.13</v>
       </c>
-      <c r="L28">
+      <c r="M28">
         <v>21886.93</v>
       </c>
-      <c r="M28">
+      <c r="N28">
         <v>28.5</v>
       </c>
-      <c r="N28">
+      <c r="O28">
         <v>27</v>
       </c>
-      <c r="O28">
+      <c r="P28">
         <v>13</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>500</v>
       </c>
-      <c r="B29">
+      <c r="C29">
         <v>259.2</v>
       </c>
-      <c r="C29" t="s">
+      <c r="D29" t="s">
         <v>17</v>
       </c>
-      <c r="D29">
+      <c r="E29">
         <v>98582.5</v>
       </c>
-      <c r="E29">
+      <c r="F29">
         <v>392886.42</v>
       </c>
-      <c r="F29">
+      <c r="G29">
         <v>292237.42</v>
       </c>
-      <c r="G29">
+      <c r="H29">
         <v>100649</v>
       </c>
-      <c r="H29">
+      <c r="I29">
         <v>0</v>
       </c>
-      <c r="I29">
+      <c r="J29">
         <v>100</v>
       </c>
-      <c r="J29">
+      <c r="K29">
         <v>26</v>
       </c>
-      <c r="K29">
+      <c r="L29">
         <v>24002.98</v>
       </c>
-      <c r="L29">
+      <c r="M29">
         <v>21936.48</v>
       </c>
-      <c r="M29">
+      <c r="N29">
         <v>22.85</v>
-      </c>
-      <c r="N29">
-        <v>0</v>
       </c>
       <c r="O29">
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>100</v>
       </c>
-      <c r="B30">
+      <c r="C30">
         <v>194.4</v>
       </c>
-      <c r="C30" t="s">
+      <c r="D30" t="s">
         <v>17</v>
       </c>
-      <c r="D30">
+      <c r="E30">
         <v>98582.5</v>
       </c>
-      <c r="E30">
+      <c r="F30">
         <v>294664.96000000002</v>
       </c>
-      <c r="F30">
+      <c r="G30">
         <v>197596.82</v>
       </c>
-      <c r="G30">
+      <c r="H30">
         <v>97068.14</v>
       </c>
-      <c r="H30">
+      <c r="I30">
         <v>3321.05</v>
       </c>
-      <c r="I30">
+      <c r="J30">
         <v>97</v>
       </c>
-      <c r="J30">
+      <c r="K30">
         <v>33</v>
       </c>
-      <c r="K30">
+      <c r="L30">
         <v>23208.720000000001</v>
       </c>
-      <c r="L30">
+      <c r="M30">
         <v>21402.04</v>
       </c>
-      <c r="M30">
+      <c r="N30">
         <v>111.4</v>
       </c>
-      <c r="N30">
+      <c r="O30">
         <v>1469</v>
       </c>
-      <c r="O30">
+      <c r="P30">
         <v>23</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>200</v>
       </c>
-      <c r="B31">
+      <c r="C31">
         <v>194.4</v>
       </c>
-      <c r="C31" t="s">
+      <c r="D31" t="s">
         <v>17</v>
       </c>
-      <c r="D31">
+      <c r="E31">
         <v>98582.5</v>
       </c>
-      <c r="E31">
+      <c r="F31">
         <v>294664.96000000002</v>
       </c>
-      <c r="F31">
+      <c r="G31">
         <v>194605.62</v>
       </c>
-      <c r="G31">
+      <c r="H31">
         <v>100059.34</v>
       </c>
-      <c r="H31">
+      <c r="I31">
         <v>612.35</v>
       </c>
-      <c r="I31">
+      <c r="J31">
         <v>99</v>
       </c>
-      <c r="J31">
+      <c r="K31">
         <v>34</v>
       </c>
-      <c r="K31">
+      <c r="L31">
         <v>26199.93</v>
       </c>
-      <c r="L31">
+      <c r="M31">
         <v>24110.73</v>
       </c>
-      <c r="M31">
+      <c r="N31">
         <v>62.79</v>
       </c>
-      <c r="N31">
+      <c r="O31">
         <v>188</v>
       </c>
-      <c r="O31">
+      <c r="P31">
         <v>18</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>300</v>
       </c>
-      <c r="B32">
+      <c r="C32">
         <v>194.4</v>
       </c>
-      <c r="C32" t="s">
+      <c r="D32" t="s">
         <v>17</v>
       </c>
-      <c r="D32">
+      <c r="E32">
         <v>98582.5</v>
       </c>
-      <c r="E32">
+      <c r="F32">
         <v>294664.96000000002</v>
       </c>
-      <c r="F32">
+      <c r="G32">
         <v>194115.9</v>
       </c>
-      <c r="G32">
+      <c r="H32">
         <v>100549.06</v>
       </c>
-      <c r="H32">
+      <c r="I32">
         <v>209.03</v>
       </c>
-      <c r="I32">
+      <c r="J32">
         <v>100</v>
       </c>
-      <c r="J32">
+      <c r="K32">
         <v>34</v>
       </c>
-      <c r="K32">
+      <c r="L32">
         <v>26689.65</v>
       </c>
-      <c r="L32">
+      <c r="M32">
         <v>24514.05</v>
       </c>
-      <c r="M32">
+      <c r="N32">
         <v>42.56</v>
       </c>
-      <c r="N32">
+      <c r="O32">
         <v>65</v>
       </c>
-      <c r="O32">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P32">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>400</v>
       </c>
-      <c r="B33">
+      <c r="C33">
         <v>194.4</v>
       </c>
-      <c r="C33" t="s">
+      <c r="D33" t="s">
         <v>17</v>
       </c>
-      <c r="D33">
+      <c r="E33">
         <v>98582.5</v>
       </c>
-      <c r="E33">
+      <c r="F33">
         <v>294664.96000000002</v>
       </c>
-      <c r="F33">
+      <c r="G33">
         <v>193919.97</v>
       </c>
-      <c r="G33">
+      <c r="H33">
         <v>100744.99</v>
       </c>
-      <c r="H33">
+      <c r="I33">
         <v>76.459999999999994</v>
       </c>
-      <c r="I33">
+      <c r="J33">
         <v>100</v>
       </c>
-      <c r="J33">
+      <c r="K33">
         <v>34</v>
       </c>
-      <c r="K33">
+      <c r="L33">
         <v>26885.57</v>
       </c>
-      <c r="L33">
+      <c r="M33">
         <v>24646.62</v>
       </c>
-      <c r="M33">
+      <c r="N33">
         <v>32.090000000000003</v>
       </c>
-      <c r="N33">
+      <c r="O33">
         <v>28</v>
       </c>
-      <c r="O33">
+      <c r="P33">
         <v>14</v>
       </c>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>500</v>
       </c>
-      <c r="B34">
+      <c r="C34">
         <v>194.4</v>
       </c>
-      <c r="C34" t="s">
+      <c r="D34" t="s">
         <v>17</v>
       </c>
-      <c r="D34">
+      <c r="E34">
         <v>98582.5</v>
       </c>
-      <c r="E34">
+      <c r="F34">
         <v>294664.96000000002</v>
       </c>
-      <c r="F34">
+      <c r="G34">
         <v>193784.92</v>
       </c>
-      <c r="G34">
+      <c r="H34">
         <v>100880.04</v>
       </c>
-      <c r="H34">
+      <c r="I34">
         <v>0</v>
       </c>
-      <c r="I34">
+      <c r="J34">
         <v>100</v>
       </c>
-      <c r="J34">
+      <c r="K34">
         <v>34</v>
       </c>
-      <c r="K34">
+      <c r="L34">
         <v>27020.62</v>
       </c>
-      <c r="L34">
+      <c r="M34">
         <v>24723.08</v>
       </c>
-      <c r="M34">
+      <c r="N34">
         <v>25.75</v>
-      </c>
-      <c r="N34">
-        <v>0</v>
       </c>
       <c r="O34">
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>100</v>
       </c>
-      <c r="B35">
+      <c r="C35">
         <v>194.4</v>
       </c>
-      <c r="C35" t="s">
+      <c r="D35" t="s">
         <v>15</v>
       </c>
-      <c r="D35">
+      <c r="E35">
         <v>135543.5</v>
       </c>
-      <c r="E35">
+      <c r="F35">
         <v>294664.96000000002</v>
       </c>
-      <c r="F35">
+      <c r="G35">
         <v>170465.94</v>
       </c>
-      <c r="G35">
+      <c r="H35">
         <v>124199.03</v>
       </c>
-      <c r="H35">
+      <c r="I35">
         <v>13465.73</v>
       </c>
-      <c r="I35">
+      <c r="J35">
         <v>90</v>
       </c>
-      <c r="J35">
+      <c r="K35">
         <v>42</v>
       </c>
-      <c r="K35">
+      <c r="L35">
         <v>27546.65</v>
       </c>
-      <c r="L35">
+      <c r="M35">
         <v>25425.4</v>
       </c>
-      <c r="M35">
+      <c r="N35">
         <v>132.22</v>
       </c>
-      <c r="N35">
+      <c r="O35">
         <v>4225</v>
       </c>
-      <c r="O35">
+      <c r="P35">
         <v>39</v>
       </c>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>200</v>
       </c>
-      <c r="B36">
+      <c r="C36">
         <v>194.4</v>
       </c>
-      <c r="C36" t="s">
+      <c r="D36" t="s">
         <v>15</v>
       </c>
-      <c r="D36">
+      <c r="E36">
         <v>135543.5</v>
       </c>
-      <c r="E36">
+      <c r="F36">
         <v>294664.96000000002</v>
       </c>
-      <c r="F36">
+      <c r="G36">
         <v>160487.24</v>
       </c>
-      <c r="G36">
+      <c r="H36">
         <v>134177.73000000001</v>
       </c>
-      <c r="H36">
+      <c r="I36">
         <v>4273.88</v>
       </c>
-      <c r="I36">
+      <c r="J36">
         <v>97</v>
       </c>
-      <c r="J36">
+      <c r="K36">
         <v>46</v>
       </c>
-      <c r="K36">
+      <c r="L36">
         <v>37525.35</v>
       </c>
-      <c r="L36">
+      <c r="M36">
         <v>34617.25</v>
       </c>
-      <c r="M36">
+      <c r="N36">
         <v>90.06</v>
       </c>
-      <c r="N36">
+      <c r="O36">
         <v>1194</v>
       </c>
-      <c r="O36">
+      <c r="P36">
         <v>37</v>
       </c>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>300</v>
       </c>
-      <c r="B37">
+      <c r="C37">
         <v>194.4</v>
       </c>
-      <c r="C37" t="s">
+      <c r="D37" t="s">
         <v>15</v>
       </c>
-      <c r="D37">
+      <c r="E37">
         <v>135543.5</v>
       </c>
-      <c r="E37">
+      <c r="F37">
         <v>294664.96000000002</v>
       </c>
-      <c r="F37">
+      <c r="G37">
         <v>158131.73000000001</v>
       </c>
-      <c r="G37">
+      <c r="H37">
         <v>136533.23000000001</v>
       </c>
-      <c r="H37">
+      <c r="I37">
         <v>2151.04</v>
       </c>
-      <c r="I37">
+      <c r="J37">
         <v>98</v>
       </c>
-      <c r="J37">
+      <c r="K37">
         <v>46</v>
       </c>
-      <c r="K37">
+      <c r="L37">
         <v>39880.86</v>
       </c>
-      <c r="L37">
+      <c r="M37">
         <v>36740.080000000002</v>
       </c>
-      <c r="M37">
+      <c r="N37">
         <v>63.78</v>
       </c>
-      <c r="N37">
+      <c r="O37">
         <v>534</v>
       </c>
-      <c r="O37">
+      <c r="P37">
         <v>37</v>
       </c>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>400</v>
       </c>
-      <c r="B38">
+      <c r="C38">
         <v>194.4</v>
       </c>
-      <c r="C38" t="s">
+      <c r="D38" t="s">
         <v>15</v>
       </c>
-      <c r="D38">
+      <c r="E38">
         <v>135543.5</v>
       </c>
-      <c r="E38">
+      <c r="F38">
         <v>294664.96000000002</v>
       </c>
-      <c r="F38">
+      <c r="G38">
         <v>156859.29</v>
       </c>
-      <c r="G38">
+      <c r="H38">
         <v>137805.67000000001</v>
       </c>
-      <c r="H38">
+      <c r="I38">
         <v>1026.3599999999999</v>
       </c>
-      <c r="I38">
+      <c r="J38">
         <v>99</v>
       </c>
-      <c r="J38">
+      <c r="K38">
         <v>47</v>
       </c>
-      <c r="K38">
+      <c r="L38">
         <v>41153.300000000003</v>
       </c>
-      <c r="L38">
+      <c r="M38">
         <v>37864.769999999997</v>
       </c>
-      <c r="M38">
+      <c r="N38">
         <v>49.3</v>
       </c>
-      <c r="N38">
+      <c r="O38">
         <v>222</v>
       </c>
-      <c r="O38">
+      <c r="P38">
         <v>21</v>
       </c>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>500</v>
       </c>
-      <c r="B39">
+      <c r="C39">
         <v>194.4</v>
       </c>
-      <c r="C39" t="s">
+      <c r="D39" t="s">
         <v>15</v>
       </c>
-      <c r="D39">
+      <c r="E39">
         <v>135543.5</v>
       </c>
-      <c r="E39">
+      <c r="F39">
         <v>294664.96000000002</v>
       </c>
-      <c r="F39">
+      <c r="G39">
         <v>156218.21</v>
       </c>
-      <c r="G39">
+      <c r="H39">
         <v>138446.76</v>
       </c>
-      <c r="H39">
+      <c r="I39">
         <v>483.54</v>
       </c>
-      <c r="I39">
+      <c r="J39">
         <v>100</v>
       </c>
-      <c r="J39">
+      <c r="K39">
         <v>47</v>
       </c>
-      <c r="K39">
+      <c r="L39">
         <v>41794.379999999997</v>
       </c>
-      <c r="L39">
+      <c r="M39">
         <v>38407.589999999997</v>
       </c>
-      <c r="M39">
+      <c r="N39">
         <v>40.01</v>
       </c>
-      <c r="N39">
+      <c r="O39">
         <v>103</v>
       </c>
-      <c r="O39">
+      <c r="P39">
         <v>18</v>
       </c>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>600</v>
       </c>
-      <c r="B40">
+      <c r="C40">
         <v>194.4</v>
       </c>
-      <c r="C40" t="s">
+      <c r="D40" t="s">
         <v>15</v>
       </c>
-      <c r="D40">
+      <c r="E40">
         <v>135543.5</v>
       </c>
-      <c r="E40">
+      <c r="F40">
         <v>294664.96000000002</v>
       </c>
-      <c r="F40">
+      <c r="G40">
         <v>155936.12</v>
       </c>
-      <c r="G40">
+      <c r="H40">
         <v>138728.84</v>
       </c>
-      <c r="H40">
+      <c r="I40">
         <v>271.57</v>
       </c>
-      <c r="I40">
+      <c r="J40">
         <v>100</v>
       </c>
-      <c r="J40">
+      <c r="K40">
         <v>47</v>
       </c>
-      <c r="K40">
+      <c r="L40">
         <v>42076.47</v>
       </c>
-      <c r="L40">
+      <c r="M40">
         <v>38619.56</v>
       </c>
-      <c r="M40">
+      <c r="N40">
         <v>33.520000000000003</v>
       </c>
-      <c r="N40">
+      <c r="O40">
         <v>34</v>
       </c>
-      <c r="O40">
+      <c r="P40">
         <v>17</v>
       </c>
     </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>700</v>
       </c>
-      <c r="B41">
+      <c r="C41">
         <v>194.4</v>
       </c>
-      <c r="C41" t="s">
+      <c r="D41" t="s">
         <v>15</v>
       </c>
-      <c r="D41">
+      <c r="E41">
         <v>135543.5</v>
       </c>
-      <c r="E41">
+      <c r="F41">
         <v>294664.96000000002</v>
       </c>
-      <c r="F41">
+      <c r="G41">
         <v>155790.28</v>
       </c>
-      <c r="G41">
+      <c r="H41">
         <v>138874.68</v>
       </c>
-      <c r="H41">
+      <c r="I41">
         <v>185.17</v>
       </c>
-      <c r="I41">
+      <c r="J41">
         <v>100</v>
       </c>
-      <c r="J41">
+      <c r="K41">
         <v>47</v>
       </c>
-      <c r="K41">
+      <c r="L41">
         <v>42222.31</v>
       </c>
-      <c r="L41">
+      <c r="M41">
         <v>38705.96</v>
       </c>
-      <c r="M41">
+      <c r="N41">
         <v>28.8</v>
       </c>
-      <c r="N41">
+      <c r="O41">
         <v>31</v>
       </c>
-      <c r="O41">
+      <c r="P41">
         <v>15</v>
       </c>
     </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>800</v>
       </c>
-      <c r="B42">
+      <c r="C42">
         <v>194.4</v>
       </c>
-      <c r="C42" t="s">
+      <c r="D42" t="s">
         <v>15</v>
       </c>
-      <c r="D42">
+      <c r="E42">
         <v>135543.5</v>
       </c>
-      <c r="E42">
+      <c r="F42">
         <v>294664.96000000002</v>
       </c>
-      <c r="F42">
+      <c r="G42">
         <v>155644.45000000001</v>
       </c>
-      <c r="G42">
+      <c r="H42">
         <v>139020.51</v>
       </c>
-      <c r="H42">
+      <c r="I42">
         <v>98.77</v>
       </c>
-      <c r="I42">
+      <c r="J42">
         <v>100</v>
       </c>
-      <c r="J42">
+      <c r="K42">
         <v>47</v>
       </c>
-      <c r="K42">
+      <c r="L42">
         <v>42368.14</v>
       </c>
-      <c r="L42">
+      <c r="M42">
         <v>38792.36</v>
       </c>
-      <c r="M42">
+      <c r="N42">
         <v>25.26</v>
       </c>
-      <c r="N42">
+      <c r="O42">
         <v>28</v>
       </c>
-      <c r="O42">
+      <c r="P42">
         <v>14</v>
       </c>
     </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>900</v>
       </c>
-      <c r="B43">
+      <c r="C43">
         <v>194.4</v>
       </c>
-      <c r="C43" t="s">
+      <c r="D43" t="s">
         <v>15</v>
       </c>
-      <c r="D43">
+      <c r="E43">
         <v>135543.5</v>
       </c>
-      <c r="E43">
+      <c r="F43">
         <v>294664.96000000002</v>
       </c>
-      <c r="F43">
+      <c r="G43">
         <v>155498.62</v>
       </c>
-      <c r="G43">
+      <c r="H43">
         <v>139166.34</v>
       </c>
-      <c r="H43">
+      <c r="I43">
         <v>12.37</v>
       </c>
-      <c r="I43">
+      <c r="J43">
         <v>100</v>
       </c>
-      <c r="J43">
+      <c r="K43">
         <v>47</v>
       </c>
-      <c r="K43">
+      <c r="L43">
         <v>42513.97</v>
       </c>
-      <c r="L43">
+      <c r="M43">
         <v>38878.76</v>
       </c>
-      <c r="M43">
+      <c r="N43">
         <v>22.5</v>
       </c>
-      <c r="N43">
+      <c r="O43">
         <v>9</v>
       </c>
-      <c r="O43">
+      <c r="P43">
         <v>4</v>
       </c>
     </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>1000</v>
       </c>
-      <c r="B44">
+      <c r="C44">
         <v>194.4</v>
       </c>
-      <c r="C44" t="s">
+      <c r="D44" t="s">
         <v>15</v>
       </c>
-      <c r="D44">
+      <c r="E44">
         <v>135543.5</v>
       </c>
-      <c r="E44">
+      <c r="F44">
         <v>294664.96000000002</v>
       </c>
-      <c r="F44">
+      <c r="G44">
         <v>155433.10999999999</v>
       </c>
-      <c r="G44">
+      <c r="H44">
         <v>139231.85</v>
       </c>
-      <c r="H44">
+      <c r="I44">
         <v>0</v>
       </c>
-      <c r="I44">
+      <c r="J44">
         <v>100</v>
       </c>
-      <c r="J44">
+      <c r="K44">
         <v>47</v>
       </c>
-      <c r="K44">
+      <c r="L44">
         <v>42579.48</v>
       </c>
-      <c r="L44">
+      <c r="M44">
         <v>38891.129999999997</v>
       </c>
-      <c r="M44">
+      <c r="N44">
         <v>20.260000000000002</v>
-      </c>
-      <c r="N44">
-        <v>0</v>
       </c>
       <c r="O44">
         <v>0</v>
       </c>
-    </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>100</v>
       </c>
-      <c r="B45">
+      <c r="C45">
         <v>194.4</v>
       </c>
-      <c r="C45" t="s">
-        <v>16</v>
-      </c>
-      <c r="D45">
+      <c r="D45" t="s">
+        <v>16</v>
+      </c>
+      <c r="E45">
         <v>192783.5</v>
       </c>
-      <c r="E45">
+      <c r="F45">
         <v>294664.96000000002</v>
       </c>
-      <c r="F45">
+      <c r="G45">
         <v>131747.32</v>
       </c>
-      <c r="G45">
+      <c r="H45">
         <v>162917.64000000001</v>
       </c>
-      <c r="H45">
+      <c r="I45">
         <v>32095.53</v>
       </c>
-      <c r="I45">
+      <c r="J45">
         <v>83</v>
       </c>
-      <c r="J45" s="1">
+      <c r="K45" s="1">
         <v>55</v>
       </c>
-      <c r="K45">
+      <c r="L45">
         <v>28929.5</v>
       </c>
-      <c r="L45">
+      <c r="M45">
         <v>26699.83</v>
       </c>
-      <c r="M45">
+      <c r="N45">
         <v>138.86000000000001</v>
       </c>
-      <c r="N45">
+      <c r="O45">
         <v>6203</v>
       </c>
-      <c r="O45">
+      <c r="P45">
         <v>40</v>
       </c>
     </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>200</v>
       </c>
-      <c r="B46">
+      <c r="C46">
         <v>194.4</v>
       </c>
-      <c r="C46" t="s">
-        <v>16</v>
-      </c>
-      <c r="D46">
+      <c r="D46" t="s">
+        <v>16</v>
+      </c>
+      <c r="E46">
         <v>192783.5</v>
       </c>
-      <c r="E46">
+      <c r="F46">
         <v>294664.96000000002</v>
       </c>
-      <c r="F46">
+      <c r="G46">
         <v>117687.48</v>
       </c>
-      <c r="G46">
+      <c r="H46">
         <v>176977.49</v>
       </c>
-      <c r="H46">
+      <c r="I46">
         <v>19099.580000000002</v>
       </c>
-      <c r="I46">
+      <c r="J46">
         <v>90</v>
       </c>
-      <c r="J46">
+      <c r="K46">
         <v>60</v>
       </c>
-      <c r="K46">
+      <c r="L46">
         <v>42989.34</v>
       </c>
-      <c r="L46">
+      <c r="M46">
         <v>39695.78</v>
       </c>
-      <c r="M46">
+      <c r="N46">
         <v>103.17</v>
       </c>
-      <c r="N46">
+      <c r="O46">
         <v>3690</v>
       </c>
-      <c r="O46">
+      <c r="P46">
         <v>40</v>
       </c>
     </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>300</v>
       </c>
-      <c r="B47">
+      <c r="C47">
         <v>194.4</v>
       </c>
-      <c r="C47" t="s">
-        <v>16</v>
-      </c>
-      <c r="D47">
+      <c r="D47" t="s">
+        <v>16</v>
+      </c>
+      <c r="E47">
         <v>192783.5</v>
       </c>
-      <c r="E47">
+      <c r="F47">
         <v>294664.96000000002</v>
       </c>
-      <c r="F47">
+      <c r="G47">
         <v>111958.17</v>
       </c>
-      <c r="G47">
+      <c r="H47">
         <v>182706.79</v>
       </c>
-      <c r="H47">
+      <c r="I47">
         <v>13845.35</v>
       </c>
-      <c r="I47">
+      <c r="J47">
         <v>93</v>
       </c>
-      <c r="J47">
+      <c r="K47">
         <v>62</v>
       </c>
-      <c r="K47">
+      <c r="L47">
         <v>48718.65</v>
       </c>
-      <c r="L47">
+      <c r="M47">
         <v>44950.01</v>
       </c>
-      <c r="M47">
+      <c r="N47">
         <v>77.95</v>
       </c>
-      <c r="N47">
+      <c r="O47">
         <v>2395</v>
       </c>
-      <c r="O47">
+      <c r="P47">
         <v>40</v>
       </c>
     </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>400</v>
       </c>
-      <c r="B48">
+      <c r="C48">
         <v>194.4</v>
       </c>
-      <c r="C48" t="s">
-        <v>16</v>
-      </c>
-      <c r="D48">
+      <c r="D48" t="s">
+        <v>16</v>
+      </c>
+      <c r="E48">
         <v>192783.5</v>
       </c>
-      <c r="E48">
+      <c r="F48">
         <v>294664.96000000002</v>
       </c>
-      <c r="F48">
+      <c r="G48">
         <v>108584.58</v>
       </c>
-      <c r="G48">
+      <c r="H48">
         <v>186080.38</v>
       </c>
-      <c r="H48">
+      <c r="I48">
         <v>10784.25</v>
       </c>
-      <c r="I48">
+      <c r="J48">
         <v>94</v>
       </c>
-      <c r="J48">
+      <c r="K48">
         <v>63</v>
       </c>
-      <c r="K48">
+      <c r="L48">
         <v>52092.24</v>
       </c>
-      <c r="L48">
+      <c r="M48">
         <v>48011.1</v>
       </c>
-      <c r="M48">
+      <c r="N48">
         <v>62.51</v>
       </c>
-      <c r="N48">
+      <c r="O48">
         <v>1747</v>
       </c>
-      <c r="O48">
+      <c r="P48">
         <v>40</v>
       </c>
     </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>500</v>
       </c>
-      <c r="B49">
+      <c r="C49">
         <v>194.4</v>
       </c>
-      <c r="C49" t="s">
-        <v>16</v>
-      </c>
-      <c r="D49">
+      <c r="D49" t="s">
+        <v>16</v>
+      </c>
+      <c r="E49">
         <v>192783.5</v>
       </c>
-      <c r="E49">
+      <c r="F49">
         <v>294664.96000000002</v>
       </c>
-      <c r="F49">
+      <c r="G49">
         <v>106196.5</v>
       </c>
-      <c r="G49">
+      <c r="H49">
         <v>188468.46</v>
       </c>
-      <c r="H49">
+      <c r="I49">
         <v>8631.39</v>
       </c>
-      <c r="I49">
+      <c r="J49">
         <v>96</v>
       </c>
-      <c r="J49">
+      <c r="K49">
         <v>64</v>
       </c>
-      <c r="K49">
+      <c r="L49">
         <v>54480.32</v>
       </c>
-      <c r="L49">
+      <c r="M49">
         <v>50163.96</v>
       </c>
-      <c r="M49">
+      <c r="N49">
         <v>52.25</v>
       </c>
-      <c r="N49">
+      <c r="O49">
         <v>1412</v>
       </c>
-      <c r="O49">
+      <c r="P49">
         <v>40</v>
       </c>
     </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>600</v>
       </c>
-      <c r="B50">
+      <c r="C50">
         <v>194.4</v>
       </c>
-      <c r="C50" t="s">
-        <v>16</v>
-      </c>
-      <c r="D50">
+      <c r="D50" t="s">
+        <v>16</v>
+      </c>
+      <c r="E50">
         <v>192783.5</v>
       </c>
-      <c r="E50">
+      <c r="F50">
         <v>294664.96000000002</v>
       </c>
-      <c r="F50">
+      <c r="G50">
         <v>104278.05</v>
       </c>
-      <c r="G50">
+      <c r="H50">
         <v>190386.91</v>
       </c>
-      <c r="H50">
+      <c r="I50">
         <v>6911.36</v>
       </c>
-      <c r="I50">
+      <c r="J50">
         <v>96</v>
       </c>
-      <c r="J50">
+      <c r="K50">
         <v>65</v>
       </c>
-      <c r="K50">
+      <c r="L50">
         <v>56398.77</v>
       </c>
-      <c r="L50">
+      <c r="M50">
         <v>51884</v>
       </c>
-      <c r="M50">
+      <c r="N50">
         <v>45.04</v>
       </c>
-      <c r="N50">
+      <c r="O50">
         <v>1091</v>
       </c>
-      <c r="O50">
+      <c r="P50">
         <v>40</v>
       </c>
     </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>700</v>
       </c>
-      <c r="B51">
+      <c r="C51">
         <v>194.4</v>
       </c>
-      <c r="C51" t="s">
-        <v>16</v>
-      </c>
-      <c r="D51">
+      <c r="D51" t="s">
+        <v>16</v>
+      </c>
+      <c r="E51">
         <v>192783.5</v>
       </c>
-      <c r="E51">
+      <c r="F51">
         <v>294664.96000000002</v>
       </c>
-      <c r="F51">
+      <c r="G51">
         <v>102761.42</v>
       </c>
-      <c r="G51">
+      <c r="H51">
         <v>191903.54</v>
       </c>
-      <c r="H51">
+      <c r="I51">
         <v>5561.63</v>
       </c>
-      <c r="I51">
+      <c r="J51">
         <v>97</v>
       </c>
-      <c r="J51">
+      <c r="K51">
         <v>65</v>
       </c>
-      <c r="K51">
+      <c r="L51">
         <v>57915.39</v>
       </c>
-      <c r="L51">
+      <c r="M51">
         <v>53233.73</v>
       </c>
-      <c r="M51">
+      <c r="N51">
         <v>39.61</v>
       </c>
-      <c r="N51">
+      <c r="O51">
         <v>893</v>
       </c>
-      <c r="O51">
+      <c r="P51">
         <v>39</v>
       </c>
     </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>800</v>
       </c>
-      <c r="B52">
+      <c r="C52">
         <v>194.4</v>
       </c>
-      <c r="C52" t="s">
-        <v>16</v>
-      </c>
-      <c r="D52">
+      <c r="D52" t="s">
+        <v>16</v>
+      </c>
+      <c r="E52">
         <v>192783.5</v>
       </c>
-      <c r="E52">
+      <c r="F52">
         <v>294664.96000000002</v>
       </c>
-      <c r="F52">
+      <c r="G52">
         <v>101352.38</v>
       </c>
-      <c r="G52">
+      <c r="H52">
         <v>193312.58</v>
       </c>
-      <c r="H52">
+      <c r="I52">
         <v>4311.05</v>
       </c>
-      <c r="I52">
+      <c r="J52">
         <v>98</v>
       </c>
-      <c r="J52">
+      <c r="K52">
         <v>66</v>
       </c>
-      <c r="K52">
+      <c r="L52">
         <v>59324.44</v>
       </c>
-      <c r="L52">
+      <c r="M52">
         <v>54484.31</v>
       </c>
-      <c r="M52">
+      <c r="N52">
         <v>35.47</v>
       </c>
-      <c r="N52">
+      <c r="O52">
         <v>723</v>
       </c>
-      <c r="O52">
+      <c r="P52">
         <v>38</v>
       </c>
     </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>900</v>
       </c>
-      <c r="B53">
+      <c r="C53">
         <v>194.4</v>
       </c>
-      <c r="C53" t="s">
-        <v>16</v>
-      </c>
-      <c r="D53">
+      <c r="D53" t="s">
+        <v>16</v>
+      </c>
+      <c r="E53">
         <v>192783.5</v>
       </c>
-      <c r="E53">
+      <c r="F53">
         <v>294664.96000000002</v>
       </c>
-      <c r="F53">
+      <c r="G53">
         <v>100195.47</v>
       </c>
-      <c r="G53">
+      <c r="H53">
         <v>194469.49</v>
       </c>
-      <c r="H53">
+      <c r="I53">
         <v>3292.85</v>
       </c>
-      <c r="I53">
+      <c r="J53">
         <v>98</v>
       </c>
-      <c r="J53">
+      <c r="K53">
         <v>66</v>
       </c>
-      <c r="K53">
+      <c r="L53">
         <v>60481.35</v>
       </c>
-      <c r="L53">
+      <c r="M53">
         <v>55502.51</v>
       </c>
-      <c r="M53">
+      <c r="N53">
         <v>32.119999999999997</v>
       </c>
-      <c r="N53">
+      <c r="O53">
         <v>533</v>
       </c>
-      <c r="O53">
+      <c r="P53">
         <v>30</v>
       </c>
     </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>1000</v>
       </c>
-      <c r="B54">
+      <c r="C54">
         <v>194.4</v>
       </c>
-      <c r="C54" t="s">
-        <v>16</v>
-      </c>
-      <c r="D54">
+      <c r="D54" t="s">
+        <v>16</v>
+      </c>
+      <c r="E54">
         <v>192783.5</v>
       </c>
-      <c r="E54">
+      <c r="F54">
         <v>294664.96000000002</v>
       </c>
-      <c r="F54">
+      <c r="G54">
         <v>99317.759999999995</v>
       </c>
-      <c r="G54">
+      <c r="H54">
         <v>195347.20000000001</v>
       </c>
-      <c r="H54">
+      <c r="I54">
         <v>2531.9499999999998</v>
       </c>
-      <c r="I54">
+      <c r="J54">
         <v>99</v>
       </c>
-      <c r="J54">
+      <c r="K54">
         <v>66</v>
       </c>
-      <c r="K54">
+      <c r="L54">
         <v>61359.06</v>
       </c>
-      <c r="L54">
+      <c r="M54">
         <v>56263.41</v>
       </c>
-      <c r="M54">
+      <c r="N54">
         <v>29.3</v>
       </c>
-      <c r="N54">
+      <c r="O54">
         <v>370</v>
       </c>
-      <c r="O54">
+      <c r="P54">
         <v>20</v>
       </c>
     </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>1100</v>
       </c>
-      <c r="B55">
+      <c r="C55">
         <v>194.4</v>
       </c>
-      <c r="C55" t="s">
-        <v>16</v>
-      </c>
-      <c r="D55">
+      <c r="D55" t="s">
+        <v>16</v>
+      </c>
+      <c r="E55">
         <v>192783.5</v>
       </c>
-      <c r="E55">
+      <c r="F55">
         <v>294664.96000000002</v>
       </c>
-      <c r="F55">
+      <c r="G55">
         <v>98682.9</v>
       </c>
-      <c r="G55">
+      <c r="H55">
         <v>195982.06</v>
       </c>
-      <c r="H55">
+      <c r="I55">
         <v>1994.86</v>
       </c>
-      <c r="I55">
+      <c r="J55">
         <v>99</v>
       </c>
-      <c r="J55">
+      <c r="K55">
         <v>67</v>
       </c>
-      <c r="K55">
+      <c r="L55">
         <v>61993.919999999998</v>
       </c>
-      <c r="L55">
+      <c r="M55">
         <v>56800.5</v>
       </c>
-      <c r="M55">
+      <c r="N55">
         <v>26.89</v>
       </c>
-      <c r="N55">
+      <c r="O55">
         <v>286</v>
       </c>
-      <c r="O55">
+      <c r="P55">
         <v>20</v>
       </c>
     </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>1200</v>
       </c>
-      <c r="B56">
+      <c r="C56">
         <v>194.4</v>
       </c>
-      <c r="C56" t="s">
-        <v>16</v>
-      </c>
-      <c r="D56">
+      <c r="D56" t="s">
+        <v>16</v>
+      </c>
+      <c r="E56">
         <v>192783.5</v>
       </c>
-      <c r="E56">
+      <c r="F56">
         <v>294664.96000000002</v>
       </c>
-      <c r="F56">
+      <c r="G56">
         <v>98213.9</v>
       </c>
-      <c r="G56">
+      <c r="H56">
         <v>196451.06</v>
       </c>
-      <c r="H56">
+      <c r="I56">
         <v>1610.63</v>
       </c>
-      <c r="I56">
+      <c r="J56">
         <v>99</v>
       </c>
-      <c r="J56">
+      <c r="K56">
         <v>67</v>
       </c>
-      <c r="K56">
+      <c r="L56">
         <v>62462.92</v>
       </c>
-      <c r="L56">
+      <c r="M56">
         <v>57184.72</v>
       </c>
-      <c r="M56">
+      <c r="N56">
         <v>24.82</v>
       </c>
-      <c r="N56">
+      <c r="O56">
         <v>201</v>
       </c>
-      <c r="O56">
+      <c r="P56">
         <v>18</v>
       </c>
     </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>1300</v>
       </c>
-      <c r="B57">
+      <c r="C57">
         <v>194.4</v>
       </c>
-      <c r="C57" t="s">
-        <v>16</v>
-      </c>
-      <c r="D57">
+      <c r="D57" t="s">
+        <v>16</v>
+      </c>
+      <c r="E57">
         <v>192783.5</v>
       </c>
-      <c r="E57">
+      <c r="F57">
         <v>294664.96000000002</v>
       </c>
-      <c r="F57">
+      <c r="G57">
         <v>97838.9</v>
       </c>
-      <c r="G57">
+      <c r="H57">
         <v>196826.06</v>
       </c>
-      <c r="H57">
+      <c r="I57">
         <v>1313.03</v>
       </c>
-      <c r="I57">
+      <c r="J57">
         <v>99</v>
       </c>
-      <c r="J57">
+      <c r="K57">
         <v>67</v>
       </c>
-      <c r="K57">
+      <c r="L57">
         <v>62837.919999999998</v>
       </c>
-      <c r="L57">
+      <c r="M57">
         <v>57482.32</v>
       </c>
-      <c r="M57">
+      <c r="N57">
         <v>23.03</v>
       </c>
-      <c r="N57">
+      <c r="O57">
         <v>190</v>
       </c>
-      <c r="O57">
+      <c r="P57">
         <v>17</v>
       </c>
     </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>1400</v>
       </c>
-      <c r="B58">
+      <c r="C58">
         <v>194.4</v>
       </c>
-      <c r="C58" t="s">
-        <v>16</v>
-      </c>
-      <c r="D58">
+      <c r="D58" t="s">
+        <v>16</v>
+      </c>
+      <c r="E58">
         <v>192783.5</v>
       </c>
-      <c r="E58">
+      <c r="F58">
         <v>294664.96000000002</v>
       </c>
-      <c r="F58">
+      <c r="G58">
         <v>97463.9</v>
       </c>
-      <c r="G58">
+      <c r="H58">
         <v>197201.06</v>
       </c>
-      <c r="H58">
+      <c r="I58">
         <v>1015.43</v>
       </c>
-      <c r="I58">
+      <c r="J58">
         <v>99</v>
       </c>
-      <c r="J58">
+      <c r="K58">
         <v>67</v>
       </c>
-      <c r="K58">
+      <c r="L58">
         <v>63212.92</v>
       </c>
-      <c r="L58">
+      <c r="M58">
         <v>57779.92</v>
       </c>
-      <c r="M58">
+      <c r="N58">
         <v>21.5</v>
       </c>
-      <c r="N58">
+      <c r="O58">
         <v>156</v>
       </c>
-      <c r="O58">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P58">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="59" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>1500</v>
       </c>
-      <c r="B59">
+      <c r="C59">
         <v>194.4</v>
       </c>
-      <c r="C59" t="s">
-        <v>16</v>
-      </c>
-      <c r="D59">
+      <c r="D59" t="s">
+        <v>16</v>
+      </c>
+      <c r="E59">
         <v>192783.5</v>
       </c>
-      <c r="E59">
+      <c r="F59">
         <v>294664.96000000002</v>
       </c>
-      <c r="F59">
+      <c r="G59">
         <v>97088.9</v>
       </c>
-      <c r="G59">
+      <c r="H59">
         <v>197576.06</v>
       </c>
-      <c r="H59">
+      <c r="I59">
         <v>717.83</v>
       </c>
-      <c r="I59">
+      <c r="J59">
         <v>100</v>
       </c>
-      <c r="J59">
+      <c r="K59">
         <v>67</v>
       </c>
-      <c r="K59">
+      <c r="L59">
         <v>63587.92</v>
       </c>
-      <c r="L59">
+      <c r="M59">
         <v>58077.52</v>
       </c>
-      <c r="M59">
+      <c r="N59">
         <v>20.170000000000002</v>
       </c>
-      <c r="N59">
+      <c r="O59">
         <v>147</v>
       </c>
-      <c r="O59">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P59">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="60" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>1600</v>
       </c>
-      <c r="B60">
+      <c r="C60">
         <v>194.4</v>
       </c>
-      <c r="C60" t="s">
-        <v>16</v>
-      </c>
-      <c r="D60">
+      <c r="D60" t="s">
+        <v>16</v>
+      </c>
+      <c r="E60">
         <v>192783.5</v>
       </c>
-      <c r="E60">
+      <c r="F60">
         <v>294664.96000000002</v>
       </c>
-      <c r="F60">
+      <c r="G60">
         <v>96729.2</v>
       </c>
-      <c r="G60">
+      <c r="H60">
         <v>197935.76</v>
       </c>
-      <c r="H60">
+      <c r="I60">
         <v>434.33</v>
       </c>
-      <c r="I60">
+      <c r="J60">
         <v>100</v>
       </c>
-      <c r="J60">
+      <c r="K60">
         <v>67</v>
       </c>
-      <c r="K60">
+      <c r="L60">
         <v>63947.62</v>
       </c>
-      <c r="L60">
+      <c r="M60">
         <v>58361.03</v>
       </c>
-      <c r="M60">
+      <c r="N60">
         <v>19</v>
       </c>
-      <c r="N60">
+      <c r="O60">
         <v>115</v>
       </c>
-      <c r="O60">
+      <c r="P60">
         <v>15</v>
       </c>
     </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>1700</v>
       </c>
-      <c r="B61">
+      <c r="C61">
         <v>194.4</v>
       </c>
-      <c r="C61" t="s">
-        <v>16</v>
-      </c>
-      <c r="D61">
+      <c r="D61" t="s">
+        <v>16</v>
+      </c>
+      <c r="E61">
         <v>192783.5</v>
       </c>
-      <c r="E61">
+      <c r="F61">
         <v>294664.96000000002</v>
       </c>
-      <c r="F61">
+      <c r="G61">
         <v>96498.77</v>
       </c>
-      <c r="G61">
+      <c r="H61">
         <v>198166.19</v>
       </c>
-      <c r="H61">
+      <c r="I61">
         <v>269.97000000000003</v>
       </c>
-      <c r="I61">
+      <c r="J61">
         <v>100</v>
       </c>
-      <c r="J61">
+      <c r="K61">
         <v>67</v>
       </c>
-      <c r="K61">
+      <c r="L61">
         <v>64178.05</v>
       </c>
-      <c r="L61">
+      <c r="M61">
         <v>58525.39</v>
       </c>
-      <c r="M61">
+      <c r="N61">
         <v>17.93</v>
       </c>
-      <c r="N61">
+      <c r="O61">
         <v>85</v>
       </c>
-      <c r="O61">
+      <c r="P61">
         <v>15</v>
       </c>
     </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>1800</v>
       </c>
-      <c r="B62">
+      <c r="C62">
         <v>194.4</v>
       </c>
-      <c r="C62" t="s">
-        <v>16</v>
-      </c>
-      <c r="D62">
+      <c r="D62" t="s">
+        <v>16</v>
+      </c>
+      <c r="E62">
         <v>192783.5</v>
       </c>
-      <c r="E62">
+      <c r="F62">
         <v>294664.96000000002</v>
       </c>
-      <c r="F62">
+      <c r="G62">
         <v>96350.5</v>
       </c>
-      <c r="G62">
+      <c r="H62">
         <v>198314.46</v>
       </c>
-      <c r="H62">
+      <c r="I62">
         <v>181.33</v>
       </c>
-      <c r="I62">
+      <c r="J62">
         <v>100</v>
       </c>
-      <c r="J62">
+      <c r="K62">
         <v>67</v>
       </c>
-      <c r="K62">
+      <c r="L62">
         <v>64326.32</v>
       </c>
-      <c r="L62">
+      <c r="M62">
         <v>58614.03</v>
       </c>
-      <c r="M62">
+      <c r="N62">
         <v>16.96</v>
       </c>
-      <c r="N62">
+      <c r="O62">
         <v>57</v>
       </c>
-      <c r="O62">
+      <c r="P62">
         <v>14</v>
       </c>
     </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>1900</v>
       </c>
-      <c r="B63">
+      <c r="C63">
         <v>194.4</v>
       </c>
-      <c r="C63" t="s">
-        <v>16</v>
-      </c>
-      <c r="D63">
+      <c r="D63" t="s">
+        <v>16</v>
+      </c>
+      <c r="E63">
         <v>192783.5</v>
       </c>
-      <c r="E63">
+      <c r="F63">
         <v>294664.96000000002</v>
       </c>
-      <c r="F63">
+      <c r="G63">
         <v>96256.75</v>
       </c>
-      <c r="G63">
+      <c r="H63">
         <v>198408.21</v>
       </c>
-      <c r="H63">
+      <c r="I63">
         <v>142.93</v>
       </c>
-      <c r="I63">
+      <c r="J63">
         <v>100</v>
       </c>
-      <c r="J63">
+      <c r="K63">
         <v>67</v>
       </c>
-      <c r="K63">
+      <c r="L63">
         <v>64420.07</v>
       </c>
-      <c r="L63">
+      <c r="M63">
         <v>58652.43</v>
       </c>
-      <c r="M63">
+      <c r="N63">
         <v>16.079999999999998</v>
       </c>
-      <c r="N63">
+      <c r="O63">
         <v>56</v>
       </c>
-      <c r="O63">
+      <c r="P63">
         <v>14</v>
       </c>
     </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>2000</v>
       </c>
-      <c r="B64">
+      <c r="C64">
         <v>194.4</v>
       </c>
-      <c r="C64" t="s">
-        <v>16</v>
-      </c>
-      <c r="D64">
+      <c r="D64" t="s">
+        <v>16</v>
+      </c>
+      <c r="E64">
         <v>192783.5</v>
       </c>
-      <c r="E64">
+      <c r="F64">
         <v>294664.96000000002</v>
       </c>
-      <c r="F64">
+      <c r="G64">
         <v>96163</v>
       </c>
-      <c r="G64">
+      <c r="H64">
         <v>198501.96</v>
       </c>
-      <c r="H64">
+      <c r="I64">
         <v>104.53</v>
       </c>
-      <c r="I64">
+      <c r="J64">
         <v>100</v>
       </c>
-      <c r="J64">
+      <c r="K64">
         <v>67</v>
       </c>
-      <c r="K64">
+      <c r="L64">
         <v>64513.82</v>
       </c>
-      <c r="L64">
+      <c r="M64">
         <v>58690.83</v>
       </c>
-      <c r="M64">
+      <c r="N64">
         <v>15.28</v>
       </c>
-      <c r="N64">
+      <c r="O64">
         <v>49</v>
       </c>
-      <c r="O64">
+      <c r="P64">
         <v>14</v>
       </c>
     </row>
-    <row r="65" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>2100</v>
       </c>
-      <c r="B65">
+      <c r="C65">
         <v>194.4</v>
       </c>
-      <c r="C65" t="s">
-        <v>16</v>
-      </c>
-      <c r="D65">
+      <c r="D65" t="s">
+        <v>16</v>
+      </c>
+      <c r="E65">
         <v>192783.5</v>
       </c>
-      <c r="E65">
+      <c r="F65">
         <v>294664.96000000002</v>
       </c>
-      <c r="F65">
+      <c r="G65">
         <v>96069.25</v>
       </c>
-      <c r="G65">
+      <c r="H65">
         <v>198595.71</v>
       </c>
-      <c r="H65">
+      <c r="I65">
         <v>66.13</v>
       </c>
-      <c r="I65">
+      <c r="J65">
         <v>100</v>
       </c>
-      <c r="J65">
+      <c r="K65">
         <v>67</v>
       </c>
-      <c r="K65">
+      <c r="L65">
         <v>64607.57</v>
       </c>
-      <c r="L65">
+      <c r="M65">
         <v>58729.23</v>
       </c>
-      <c r="M65">
+      <c r="N65">
         <v>14.57</v>
       </c>
-      <c r="N65">
+      <c r="O65">
         <v>28</v>
       </c>
-      <c r="O65">
+      <c r="P65">
         <v>14</v>
       </c>
     </row>
-    <row r="66" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>2200</v>
       </c>
-      <c r="B66">
+      <c r="C66">
         <v>194.4</v>
       </c>
-      <c r="C66" t="s">
-        <v>16</v>
-      </c>
-      <c r="D66">
+      <c r="D66" t="s">
+        <v>16</v>
+      </c>
+      <c r="E66">
         <v>192783.5</v>
       </c>
-      <c r="E66">
+      <c r="F66">
         <v>294664.96000000002</v>
       </c>
-      <c r="F66">
+      <c r="G66">
         <v>95975.5</v>
       </c>
-      <c r="G66">
+      <c r="H66">
         <v>198689.46</v>
       </c>
-      <c r="H66">
+      <c r="I66">
         <v>27.73</v>
       </c>
-      <c r="I66">
+      <c r="J66">
         <v>100</v>
       </c>
-      <c r="J66">
+      <c r="K66">
         <v>67</v>
       </c>
-      <c r="K66">
+      <c r="L66">
         <v>64701.32</v>
       </c>
-      <c r="L66">
+      <c r="M66">
         <v>58767.63</v>
       </c>
-      <c r="M66">
+      <c r="N66">
         <v>13.91</v>
       </c>
-      <c r="N66">
+      <c r="O66">
         <v>20</v>
       </c>
-      <c r="O66">
+      <c r="P66">
         <v>10</v>
       </c>
     </row>
-    <row r="67" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>2300</v>
       </c>
-      <c r="B67">
+      <c r="C67">
         <v>194.4</v>
       </c>
-      <c r="C67" t="s">
-        <v>16</v>
-      </c>
-      <c r="D67">
+      <c r="D67" t="s">
+        <v>16</v>
+      </c>
+      <c r="E67">
         <v>192783.5</v>
       </c>
-      <c r="E67">
+      <c r="F67">
         <v>294664.96000000002</v>
       </c>
-      <c r="F67">
+      <c r="G67">
         <v>95893.34</v>
       </c>
-      <c r="G67">
+      <c r="H67">
         <v>198771.62</v>
       </c>
-      <c r="H67">
+      <c r="I67">
         <v>0</v>
       </c>
-      <c r="I67">
+      <c r="J67">
         <v>100</v>
       </c>
-      <c r="J67">
+      <c r="K67">
         <v>67</v>
       </c>
-      <c r="K67">
+      <c r="L67">
         <v>64783.48</v>
       </c>
-      <c r="L67">
+      <c r="M67">
         <v>58795.360000000001</v>
       </c>
-      <c r="M67">
+      <c r="N67">
         <v>13.31</v>
       </c>
-      <c r="N67">
+      <c r="O67">
         <v>0</v>
       </c>
-      <c r="O67">
+      <c r="P67">
         <v>0</v>
       </c>
     </row>

</xml_diff>